<commit_message>
Update main_gui.py with two demos (ibm and quantum)
</commit_message>
<xml_diff>
--- a/ibm_articles.xlsx
+++ b/ibm_articles.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C167"/>
+  <dimension ref="A1:C249"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -589,7 +589,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Unlocking the power of gen AI in ERP systems</t>
+          <t>IBM awarded Customer Choice Vendor in the Gartner Peer Insights 2024 “Voice of the Customer: Cloud Database ...</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -599,14 +599,14 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmlibS5jb20vdGhvdWdodC1sZWFkZXJzaGlwL2luc3RpdHV0ZS1idXNpbmVzcy12YWx1ZS9ibG9nL3Bvd2VyLWdlbi1haS1pbi1lcnAtc3lzdGVtc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiowFodHRwczovL3d3dy5pYm0uY29tL2Jsb2cvYW5ub3VuY2VtZW50L2libS1hd2FyZGVkLWN1c3RvbWVyLWNob2ljZS12ZW5kb3ItaW4tdGhlLWdhcnRuZXItcGVlci1pbnNpZ2h0cy0yMDI0LXZvaWNlLW9mLXRoZS1jdXN0b21lci1jbG91ZC1kYXRhYmFzZS1tYW5hZ2VtZW50LXN5c3RlbXMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>IBM awarded Customer Choice Vendor in the Gartner Peer Insights 2024 “Voice of the Customer: Cloud Database ...</t>
+          <t>Unlocking the power of gen AI in ERP systems</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -616,7 +616,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiowFodHRwczovL3d3dy5pYm0uY29tL2Jsb2cvYW5ub3VuY2VtZW50L2libS1hd2FyZGVkLWN1c3RvbWVyLWNob2ljZS12ZW5kb3ItaW4tdGhlLWdhcnRuZXItcGVlci1pbnNpZ2h0cy0yMDI0LXZvaWNlLW9mLXRoZS1jdXN0b21lci1jbG91ZC1kYXRhYmFzZS1tYW5hZ2VtZW50LXN5c3RlbXMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmlibS5jb20vdGhvdWdodC1sZWFkZXJzaGlwL2luc3RpdHV0ZS1idXNpbmVzcy12YWx1ZS9ibG9nL3Bvd2VyLWdlbi1haS1pbi1lcnAtc3lzdGVtc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -657,7 +657,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>IBM Research Chief Darío Gil Chosen as Next NSB Chair</t>
+          <t>IBM and SAP unlock business and industry value with new generative AI solutions</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -667,14 +667,14 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWWh0dHBzOi8vd3d3LmhwY3dpcmUuY29tLzIwMjQvMDYvMDQvaWJtLXJlc2VhcmNoLWNoaWVmLWRhcmlvLWdpbC1jaG9zZW4tYXMtbmV4dC1uc2ItY2hhaXIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvaWJtLWFuZC1zYXAtdW5sb2NrLWJ1c2luZXNzLWFuZC1pbmR1c3RyeS12YWx1ZS13aXRoLW5ldy1nZW5lcmF0aXZlLWFpLXNvbHV0aW9ucy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Celebrating IBM Volunteer Excellence Across the World</t>
+          <t>ID Dataweb, IBM collaborate on integrating identity verification solution</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -684,14 +684,14 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiWWh0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9jZWxlYnJhdGluZy1pYm0tdm9sdW50ZWVyLWV4Y2VsbGVuY2UtYWNyb3NzLTE3MDAwMDkyMS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LmJpb21ldHJpY3VwZGF0ZS5jb20vMjAyNDA2L2lkLWRhdGF3ZWItaWJtLWNvbGxhYm9yYXRlLW9uLWludGVncmF0aW5nLWlkZW50aXR5LXZlcmlmaWNhdGlvbi1zb2x1dGlvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>NSF Board Elects IBM Executive as New Chair</t>
+          <t>IBM Research Chief Darío Gil Chosen as Next NSB Chair</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -701,14 +701,14 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3cyLmFpcC5vcmcvZnlpL25zZi1ib2FyZC1lbGVjdHMtaWJtLWV4ZWN1dGl2ZS1hcy1uZXctY2hhaXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vd3d3LmhwY3dpcmUuY29tLzIwMjQvMDYvMDQvaWJtLXJlc2VhcmNoLWNoaWVmLWRhcmlvLWdpbC1jaG9zZW4tYXMtbmV4dC1uc2ItY2hhaXIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ID Dataweb, IBM collaborate on integrating identity verification solution</t>
+          <t>Celebrating IBM Volunteer Excellence Across the World</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -718,14 +718,14 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LmJpb21ldHJpY3VwZGF0ZS5jb20vMjAyNDA2L2lkLWRhdGF3ZWItaWJtLWNvbGxhYm9yYXRlLW9uLWludGVncmF0aW5nLWlkZW50aXR5LXZlcmlmaWNhdGlvbi1zb2x1dGlvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWWh0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9jZWxlYnJhdGluZy1pYm0tdm9sdW50ZWVyLWV4Y2VsbGVuY2UtYWNyb3NzLTE3MDAwMDkyMS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>IBM and SAP unlock business and industry value with new generative AI solutions</t>
+          <t>NSF Board Elects IBM Executive as New Chair</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -735,7 +735,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvaWJtLWFuZC1zYXAtdW5sb2NrLWJ1c2luZXNzLWFuZC1pbmR1c3RyeS12YWx1ZS13aXRoLW5ldy1nZW5lcmF0aXZlLWFpLXNvbHV0aW9ucy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3cyLmFpcC5vcmcvZnlpL25zZi1ib2FyZC1lbGVjdHMtaWJtLWV4ZWN1dGl2ZS1hcy1uZXctY2hhaXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>IBM Study: Banking and Financial Markets CEOs are betting on generative AI to stay competitive, yet workforce and ...</t>
+          <t>IBM (IBM) Gains But Lags Market: What You Should Know</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -786,14 +786,14 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMi3wFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9JQk0vcHJlc3NyZWxlYXNlcy8yNjYyODUzOC9pYm0tc3R1ZHktYmFua2luZy1hbmQtZmluYW5jaWFsLW1hcmtldHMtY2Vvcy1hcmUtYmV0dGluZy1vbi1nZW5lcmF0aXZlLWFpLXRvLXN0YXktY29tcGV0aXRpdmUteWV0LXdvcmtmb3JjZS1hbmQtY3VsdHVyZS1jaGFsbGVuZ2VzLXBlcnNpc3Qv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9pYm0taWJtLWdhaW5zLWxhZ3MtbWFya2V0LTIxNDUwOTMyOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>IBM (IBM) Gains But Lags Market: What You Should Know</t>
+          <t>IBM Study: Banking and Financial Markets CEOs are betting on generative AI to stay competitive, yet workforce and ...</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -803,14 +803,14 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9pYm0taWJtLWdhaW5zLWxhZ3MtbWFya2V0LTIxNDUwOTMyOC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMi3wFodHRwczovL3d3dy50aGVnbG9iZWFuZG1haWwuY29tL2ludmVzdGluZy9tYXJrZXRzL3N0b2Nrcy9JQk0vcHJlc3NyZWxlYXNlcy8yNjYyODUzOC9pYm0tc3R1ZHktYmFua2luZy1hbmQtZmluYW5jaWFsLW1hcmtldHMtY2Vvcy1hcmUtYmV0dGluZy1vbi1nZW5lcmF0aXZlLWFpLXRvLXN0YXktY29tcGV0aXRpdmUteWV0LXdvcmtmb3JjZS1hbmQtY3VsdHVyZS1jaGFsbGVuZ2VzLXBlcnNpc3Qv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>IBM: Banking and Financial Markets CEOs are betting on AI</t>
+          <t>Scale enterprise gen AI for code generation with IBM Granite code models, available as NVIDIA NIM inference ...</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -820,14 +820,14 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZpZXJjZS1uZXR3b3JrLmNvbS9uZXdzd2lyZS9pYm0tYmFua2luZy1hbmQtZmluYW5jaWFsLW1hcmtldHMtY2Vvcy1hcmUtYmV0dGluZy1hadIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvc2NhbGUtZW50ZXJwcmlzZS1nZW4tYWktZm9yLWNvZGUtZ2VuZXJhdGlvbi13aXRoLWlibS1ncmFuaXRlLWNvZGUtbnZpZGlhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>IBM's Think 2024 News That Should Help Skills &amp; Productivity Issues in Australia</t>
+          <t>IBM: Banking and Financial Markets CEOs are betting on AI</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -837,14 +837,14 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiPmh0dHBzOi8vd3d3LnRlY2hyZXB1YmxpYy5jb20vYXJ0aWNsZS9pYm0tdGhpbmstYXVzdHJhbGlhLXRlY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmZpZXJjZS1uZXR3b3JrLmNvbS9uZXdzd2lyZS9pYm0tYmFua2luZy1hbmQtZmluYW5jaWFsLW1hcmtldHMtY2Vvcy1hcmUtYmV0dGluZy1hadIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Prioritizing operational resiliency to reduce downtime in payments</t>
+          <t>IBM's Think 2024 News That Should Help Skills &amp; Productivity Issues in Australia</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -854,14 +854,14 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9wcmlvcml0aXppbmctb3BlcmF0aW9uYWwtcmVzaWxpZW5jeS10by1yZWR1Y2UtZG93bnRpbWUtaW4tcGF5bWVudHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiPmh0dHBzOi8vd3d3LnRlY2hyZXB1YmxpYy5jb20vYXJ0aWNsZS9pYm0tdGhpbmstYXVzdHJhbGlhLXRlY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Scale enterprise gen AI for code generation with IBM Granite code models, available as NVIDIA NIM inference ...</t>
+          <t>Prioritizing operational resiliency to reduce downtime in payments</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -871,14 +871,14 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMib2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvc2NhbGUtZW50ZXJwcmlzZS1nZW4tYWktZm9yLWNvZGUtZ2VuZXJhdGlvbi13aXRoLWlibS1ncmFuaXRlLWNvZGUtbnZpZGlhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXGh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9wcmlvcml0aXppbmctb3BlcmF0aW9uYWwtcmVzaWxpZW5jeS10by1yZWR1Y2UtZG93bnRpbWUtaW4tcGF5bWVudHMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Maximizing SaaS application analytics value with AI</t>
+          <t>This AI skill pays over $100,000 a year and is in 'crazy demand,' says IBM exec—it's one 'you can use almost anywhere'</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -888,14 +888,14 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiL2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hcHBsaWNhdGlvbi1hbmFseXRpY3Mv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjQvMDYvMDUvYWktc2tpbGwtaW4tY3JhenktZGVtYW5kLXBheXMtb3Zlci0xMDAwMDAtZG9sbGFycy1hLXllYXIuaHRtbNIBYWh0dHBzOi8vd3d3LmNuYmMuY29tL2FtcC8yMDI0LzA2LzA1L2FpLXNraWxsLWluLWNyYXp5LWRlbWFuZC1wYXlzLW92ZXItMTAwMDAwLWRvbGxhcnMtYS15ZWFyLmh0bWw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>This AI skill pays over $100,000 a year and is in 'crazy demand,' says IBM exec—it's one 'you can use almost anywhere'</t>
+          <t>Q-CTRL solves IBM quantum computer problem</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -905,14 +905,14 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmNuYmMuY29tLzIwMjQvMDYvMDUvYWktc2tpbGwtaW4tY3JhenktZGVtYW5kLXBheXMtb3Zlci0xMDAwMDAtZG9sbGFycy1hLXllYXIuaHRtbNIBYWh0dHBzOi8vd3d3LmNuYmMuY29tL2FtcC8yMDI0LzA2LzA1L2FpLXNraWxsLWluLWNyYXp5LWRlbWFuZC1wYXlzLW92ZXItMTAwMDAwLWRvbGxhcnMtYS15ZWFyLmh0bWw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmZ1ZHppbGxhLmNvbS9uZXdzLzU5MTEyLXEtY3RybC1zb2x2ZXMtaWJtLXF1YW50dW0tY29tcHV0ZXItcHJvYmxlbdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Q-CTRL solves IBM quantum computer problem</t>
+          <t>Rapidus, IBM expand collaboration to chiplet packaging technology - TipRanks.com</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -922,14 +922,14 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3LmZ1ZHppbGxhLmNvbS9uZXdzLzU5MTEyLXEtY3RybC1zb2x2ZXMtaWJtLXF1YW50dW0tY29tcHV0ZXItcHJvYmxlbdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LnRpcHJhbmtzLmNvbS9uZXdzL3RoZS1mbHkvcmFwaWR1cy1pYm0tZXhwYW5kLWNvbGxhYm9yYXRpb24tdG8tY2hpcGxldC1wYWNrYWdpbmctdGVjaG5vbG9nedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Rapidus, IBM expand collaboration to chiplet packaging technology - TipRanks.com</t>
+          <t>Maximizing SaaS application analytics value with AI</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -939,14 +939,14 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LnRpcHJhbmtzLmNvbS9uZXdzL3RoZS1mbHkvcmFwaWR1cy1pYm0tZXhwYW5kLWNvbGxhYm9yYXRpb24tdG8tY2hpcGxldC1wYWNrYWdpbmctdGVjaG5vbG9nedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiL2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hcHBsaWNhdGlvbi1hbmFseXRpY3Mv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>IBM and Pasqal Initiate Collaboration to Define Classical-Quantum Integration for Quantum-Centric Supercomputers</t>
+          <t>IBM Think 2024: Making AI Real For Enterprises</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -956,14 +956,14 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMilAFodHRwczovL25ld3Nyb29tLmlibS5jb20vMjAyNC0wNi0wNi1JQk0tYW5kLVBhc3FhbC1Jbml0aWF0ZS1Db2xsYWJvcmF0aW9uLXRvLURlZmluZS1DbGFzc2ljYWwtUXVhbnR1bS1JbnRlZ3JhdGlvbi1mb3ItUXVhbnR1bS1DZW50cmljLVN1cGVyY29tcHV0ZXJz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvcGF0cmlja21vb3JoZWFkLzIwMjQvMDYvMDYvaWJtLXRoaW5rLTIwMjQtbWFraW5nLWFpLXJlYWwtZm9yLWVudGVycHJpc2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Clinic, IBM and Hartree to Advance Healthcare with AI</t>
+          <t>IBM, Pasqal to Partner on Quantum-Centric Supercomputing</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -973,14 +973,14 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMixQFodHRwczovL25ld3Nyb29tLmNsZXZlbGFuZGNsaW5pYy5vcmcvMjAyNC8wNi8wNi9jbGV2ZWxhbmQtY2xpbmljLWlibS1hbmQtdGhlLWhhcnRyZWUtY2VudHJlLWNvbGxhYm9yYXRlLXRvLWFkdmFuY2UtaGVhbHRoY2FyZS1hbmQtbGlmZS1zY2llbmNlcy10aHJvdWdoLWFydGlmaWNpYWwtaW50ZWxsaWdlbmNlLWFuZC1xdWFudHVtLWNvbXB1dGluZ9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vaWJtLXBhc3FhbC10by1wYXJ0bmVyLW9uLXF1YW50dW0tY2VudHJpYy1zdXBlcmNvbXB1dGluZ9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Empowering Women and Girls in Asia-Pacific: IBM's commitment to education</t>
+          <t>Palo Alto Networks Buys IBM QRadar</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -990,14 +990,14 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbmV3c3Jvb20uaWJtLmNvbS9CbG9nLUVtcG93ZXJpbmctV29tZW4tYW5kLUdpcmxzLWluLUFzaWEtUGFjaWZpYy1JQk1zLWNvbW1pdG1lbnQtdG8tZWR1Y2F0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3Lm1zc3BhbGVydC5jb20vbmV3cy9wYWxvLWFsdG8tbmV0d29ya3MtaWJtLXFyYWRhci1idXktc3BhcmtzLW1zc3AtbXNwLW9wcG9ydHVuaXRpZXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Palo Alto Networks Buys IBM QRadar</t>
+          <t>Clinic, IBM and Hartree to Advance Healthcare with AI</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1007,14 +1007,14 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXmh0dHBzOi8vd3d3Lm1zc3BhbGVydC5jb20vbmV3cy9wYWxvLWFsdG8tbmV0d29ya3MtaWJtLXFyYWRhci1idXktc3BhcmtzLW1zc3AtbXNwLW9wcG9ydHVuaXRpZXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMixQFodHRwczovL25ld3Nyb29tLmNsZXZlbGFuZGNsaW5pYy5vcmcvMjAyNC8wNi8wNi9jbGV2ZWxhbmQtY2xpbmljLWlibS1hbmQtdGhlLWhhcnRyZWUtY2VudHJlLWNvbGxhYm9yYXRlLXRvLWFkdmFuY2UtaGVhbHRoY2FyZS1hbmQtbGlmZS1zY2llbmNlcy10aHJvdWdoLWFydGlmaWNpYWwtaW50ZWxsaWdlbmNlLWFuZC1xdWFudHVtLWNvbXB1dGluZ9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>IBM, Pasqal to Partner on Quantum-Centric Supercomputing</t>
+          <t>IBM and Pasqal Initiate Collaboration to Define Classical-Quantum Integration for Quantum-Centric Supercomputers</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1024,14 +1024,14 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vaWJtLXBhc3FhbC10by1wYXJ0bmVyLW9uLXF1YW50dW0tY2VudHJpYy1zdXBlcmNvbXB1dGluZ9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMilAFodHRwczovL25ld3Nyb29tLmlibS5jb20vMjAyNC0wNi0wNi1JQk0tYW5kLVBhc3FhbC1Jbml0aWF0ZS1Db2xsYWJvcmF0aW9uLXRvLURlZmluZS1DbGFzc2ljYWwtUXVhbnR1bS1JbnRlZ3JhdGlvbi1mb3ItUXVhbnR1bS1DZW50cmljLVN1cGVyY29tcHV0ZXJz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>IBM Think 2024: Making AI Real For Enterprises</t>
+          <t>Empowering Women and Girls in Asia-Pacific: IBM's commitment to education</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1041,14 +1041,14 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmZvcmJlcy5jb20vc2l0ZXMvcGF0cmlja21vb3JoZWFkLzIwMjQvMDYvMDYvaWJtLXRoaW5rLTIwMjQtbWFraW5nLWFpLXJlYWwtZm9yLWVudGVycHJpc2VzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vbmV3c3Jvb20uaWJtLmNvbS9CbG9nLUVtcG93ZXJpbmctV29tZW4tYW5kLUdpcmxzLWluLUFzaWEtUGFjaWZpYy1JQk1zLWNvbW1pdG1lbnQtdG8tZWR1Y2F0aW9u0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HashiCorp stock downgraded by JMP Securities, cites IBM acquisition agreement By Investing.com</t>
+          <t>IBM and Pasqal Collaborate on Classical-Quantum Integration for Supercomputers</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1058,14 +1058,14 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5pbnZlc3RpbmcuY29tL25ld3MvY29tcGFueS1uZXdzL2hhc2hpY29ycC1zdG9jay1kb3duZ3JhZGVkLWJ5LWptcC1zZWN1cml0aWVzLWNpdGVzLWlibS1hY3F1aXNpdGlvbi1hZ3JlZW1lbnQtOTNDSC0zNDczMDA30gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vaWJtLWFuZC1wYXNxYWwtY29sbGFib3JhdGUtb24tY2xhc3NpY2FsLXF1YW50dW0taW50ZWdyYXRpb24tZm9yLXN1cGVyY29tcHV0ZXJzL9IBdmh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vaWJtLWFuZC1wYXNxYWwtY29sbGFib3JhdGUtb24tY2xhc3NpY2FsLXF1YW50dW0taW50ZWdyYXRpb24tZm9yLXN1cGVyY29tcHV0ZXJzL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>IBM's A Boy And His Atom Is Literally The Smallest Film Ever</t>
+          <t>IBM and Veridium to Transform Carbon Credits into Blockchain-Based Tokens</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1075,14 +1075,14 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LmdpYW50ZnJlYWtpbnJvYm90LmNvbS9zY2kvaWJtcy1ib3ktYXRvbS1saXRlcmFsbHktc21hbGxlc3QtZmlsbS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdWsubW92aWVzLnlhaG9vLmNvbS9tb3ZpZXMvaWJtLXZlcmlkaXVtLXRyYW5zZm9ybS1jYXJib24tY3JlZGl0cy0xOTQzMzU0NjEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>IBM &amp; Pasqal partner to advance quantum-centric computing</t>
+          <t>How IBM Australia Is Supporting Partners in Transformation</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1092,14 +1092,14 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiU2h0dHBzOi8vaXRicmllZi5jby5uei9zdG9yeS9pYm0tcGFzcWFsLXBhcnRuZXItdG8tYWR2YW5jZS1xdWFudHVtLWNlbnRyaWMtY29tcHV0aW5n0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmNoYW5uZWxpbnNpZGVyLmNvbS9uZXdzLWFuZC10cmVuZHMvYXBhYy9pYm0tYXVzdHJhbGlhLXN1cHBvcnQtcHJvZ3JhbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>IBM and Veridium to Transform Carbon Credits into Blockchain-Based Tokens</t>
+          <t>IBM's A Boy And His Atom Is Literally The Smallest Film Ever</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1109,14 +1109,14 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vdWsubW92aWVzLnlhaG9vLmNvbS9tb3ZpZXMvaWJtLXZlcmlkaXVtLXRyYW5zZm9ybS1jYXJib24tY3JlZGl0cy0xOTQzMzU0NjEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vd3d3LmdpYW50ZnJlYWtpbnJvYm90LmNvbS9zY2kvaWJtcy1ib3ktYXRvbS1saXRlcmFsbHktc21hbGxlc3QtZmlsbS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>IBM and Pasqal Collaborate on Classical-Quantum Integration for Supercomputers</t>
+          <t>HashiCorp stock downgraded by JMP Securities, cites IBM acquisition agreement By Investing.com</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1126,14 +1126,14 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vaWJtLWFuZC1wYXNxYWwtY29sbGFib3JhdGUtb24tY2xhc3NpY2FsLXF1YW50dW0taW50ZWdyYXRpb24tZm9yLXN1cGVyY29tcHV0ZXJzL9IBdmh0dHBzOi8vcXVhbnR1bWNvbXB1dGluZ3JlcG9ydC5jb20vaWJtLWFuZC1wYXNxYWwtY29sbGFib3JhdGUtb24tY2xhc3NpY2FsLXF1YW50dW0taW50ZWdyYXRpb24tZm9yLXN1cGVyY29tcHV0ZXJzL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5pbnZlc3RpbmcuY29tL25ld3MvY29tcGFueS1uZXdzL2hhc2hpY29ycC1zdG9jay1kb3duZ3JhZGVkLWJ5LWptcC1zZWN1cml0aWVzLWNpdGVzLWlibS1hY3F1aXNpdGlvbi1hZ3JlZW1lbnQtOTNDSC0zNDczMDA30gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>How IBM Australia Is Supporting Partners in Transformation</t>
+          <t>IBM &amp; Pasqal partner to advance quantum-centric computing</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1143,14 +1143,14 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmNoYW5uZWxpbnNpZGVyLmNvbS9uZXdzLWFuZC10cmVuZHMvYXBhYy9pYm0tYXVzdHJhbGlhLXN1cHBvcnQtcHJvZ3JhbS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiU2h0dHBzOi8vaXRicmllZi5jby5uei9zdG9yeS9pYm0tcGFzcWFsLXBhcnRuZXItdG8tYWR2YW5jZS1xdWFudHVtLWNlbnRyaWMtY29tcHV0aW5n0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Optimize your call center operations with new IBM watsonx assistants features</t>
+          <t>IBM Think 2024: Could AI Help Figure Out What Customers Will Want?</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1160,14 +1160,14 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvb3B0aW1pemUteW91ci1jYWxsLWNlbnRlci1vcGVyYXRpb25zLXdpdGgtbmV3LWlibS13YXRzb254LWFzc2lzdGFudC1mZWF0dXJlcy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vdGVjaHNwZWN0aXZlLm5ldC8yMDI0LzA2LzA3L2libS10aGluay0yMDI0LWNvdWxkLWFpLWhlbHAtZmlndXJlLW91dC13aGF0LWN1c3RvbWVycy13aWxsLXdhbnQv0gFpaHR0cHM6Ly90ZWNoc3BlY3RpdmUubmV0LzIwMjQvMDYvMDcvaWJtLXRoaW5rLTIwMjQtY291bGQtYWktaGVscC1maWd1cmUtb3V0LXdoYXQtY3VzdG9tZXJzLXdpbGwtd2FudC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>IBM Think 2024: Could AI Help Figure Out What Customers Will Want?</t>
+          <t>Optimize your call center operations with new IBM watsonx assistants features</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1177,14 +1177,14 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZWh0dHBzOi8vdGVjaHNwZWN0aXZlLm5ldC8yMDI0LzA2LzA3L2libS10aGluay0yMDI0LWNvdWxkLWFpLWhlbHAtZmlndXJlLW91dC13aGF0LWN1c3RvbWVycy13aWxsLXdhbnQv0gFpaHR0cHM6Ly90ZWNoc3BlY3RpdmUubmV0LzIwMjQvMDYvMDcvaWJtLXRoaW5rLTIwMjQtY291bGQtYWktaGVscC1maWd1cmUtb3V0LXdoYXQtY3VzdG9tZXJzLXdpbGwtd2FudC9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvb3B0aW1pemUteW91ci1jYWxsLWNlbnRlci1vcGVyYXRpb25zLXdpdGgtbmV3LWlibS13YXRzb254LWFzc2lzdGFudC1mZWF0dXJlcy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>IBM watsonx: New Technology Powers Sustainability Progress</t>
+          <t>A new way to collaboratively customize LLMs</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1194,14 +1194,14 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vdGVjaG5vbG9neW1hZ2F6aW5lLmNvbS9kYXRhLWFuZC1kYXRhLWFuYWx5dGljcy9pYm0td2F0c29ueC1uZXctdGVjaG5vbG9neS1wb3dlcnMtc3VzdGFpbmFiaWxpdHktcHJvZ3Jlc3PSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiKmh0dHBzOi8vcmVzZWFyY2guaWJtLmNvbS9ibG9nL2luc3RydWN0LWxhYtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>A new way to collaboratively customize LLMs</t>
+          <t>IBM watsonx: New Technology Powers Sustainability Progress</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiKmh0dHBzOi8vcmVzZWFyY2guaWJtLmNvbS9ibG9nL2luc3RydWN0LWxhYtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicGh0dHBzOi8vdGVjaG5vbG9neW1hZ2F6aW5lLmNvbS9kYXRhLWFuZC1kYXRhLWFuYWx5dGljcy9pYm0td2F0c29ueC1uZXctdGVjaG5vbG9neS1wb3dlcnMtc3VzdGFpbmFiaWxpdHktcHJvZ3Jlc3PSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1303,7 +1303,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>(IBM) Trading Advice</t>
+          <t>IBM and Red Hat Introduce InstructLab for Collaborative LLM Customization</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1313,14 +1313,14 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vbmV3cy5zdG9ja3RyYWRlcnNkYWlseS5jb20vbmV3c19yZWxlYXNlLzIxLyUyOElCTSUyOStUcmFkaW5nK0FkdmljZV8wNjA4MjQxMTM0MDIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vYmxvY2tjaGFpbi5uZXdzL25ld3MvaWJtLXJlZC1oYXQtaW5zdHJ1Y3RsYWItbGxtLWN1c3RvbWl6YXRpb27SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>International Business Machines Co. (NYSE:IBM) Receives Average Recommendation of "Hold" from Brokerages</t>
+          <t>(IBM) Trading Advice</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1330,14 +1330,14 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLWNvbnNlbnN1cy1hbmFseXN0LXJhdGluZy0yMDI0LTA2LTA4L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vbmV3cy5zdG9ja3RyYWRlcnNkYWlseS5jb20vbmV3c19yZWxlYXNlLzIxLyUyOElCTSUyOStUcmFkaW5nK0FkdmljZV8wNjA4MjQxMTM0MDIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>IBM and Red Hat Introduce InstructLab for Collaborative LLM Customization</t>
+          <t>International Business Machines Co. (NYSE:IBM) Receives Average Recommendation of "Hold" from Brokerages</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1347,7 +1347,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vYmxvY2tjaGFpbi5uZXdzL25ld3MvaWJtLXJlZC1oYXQtaW5zdHJ1Y3RsYWItbGxtLWN1c3RvbWl6YXRpb27SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLWNvbnNlbnN1cy1hbmFseXN0LXJhdGluZy0yMDI0LTA2LTA4L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1388,7 +1388,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>18448 Shares in International Business Machines Co. (NYSE:IBM) Acquired by 1832 Asset Management L.P.</t>
+          <t>International Business Machines Co. (NYSE:IBM) Shares Bought by State of Tennessee Treasury Department</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1398,14 +1398,14 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMDkvMTg0NDgtc2hhcmVzLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS1hY3F1aXJlZC1ieS0xODMyLWFzc2V0LW1hbmFnZW1lbnQtbC1wLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXNlYy1maWxpbmctMjAyNC0wNi0wOS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>International Business Machines Co. (NYSE:IBM) Shares Bought by State of Tennessee Treasury Department</t>
+          <t>18448 Shares in International Business Machines Co. (NYSE:IBM) Acquired by 1832 Asset Management L.P.</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1415,7 +1415,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXNlYy1maWxpbmctMjAyNC0wNi0wOS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMDkvMTg0NDgtc2hhcmVzLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS1hY3F1aXJlZC1ieS0xODMyLWFzc2V0LW1hbmFnZW1lbnQtbC1wLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1473,7 +1473,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Elon Musk's top 5 personality traits, according to an IBM supercomputer</t>
+          <t>Remembering Bob Dennard, inventor of the DRAM chip</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1483,14 +1483,14 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9lbG9uLW11c2stdG9wLTUtcGVyc29uYWxpdHktMTgzMjE3MDAxLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNWh0dHBzOi8vcmVzZWFyY2guaWJtLmNvbS9ibG9nL2JvYi1kZW5uYXJkLWluLW1lbW9yaWFt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Remembering Bob Dennard, inventor of the DRAM chip</t>
+          <t>Elon Musk's top 5 personality traits, according to an IBM supercomputer</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1500,7 +1500,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiNWh0dHBzOi8vcmVzZWFyY2guaWJtLmNvbS9ibG9nL2JvYi1kZW5uYXJkLWluLW1lbW9yaWFt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vY2EubW92aWVzLnlhaG9vLmNvbS9lbG9uLW11c2stdG9wLTUtcGVyc29uYWxpdHktMTgzMjE3MDAxLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -1524,7 +1524,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>IBM UK and Ireland CEO Says AI Boosting Productivity</t>
+          <t>Seven top central processing unit (CPU) use cases</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1534,14 +1534,14 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy92aWRlb3MvMjAyNC0wNi0xMC9pYm0tdWstYW5kLWlyZWxhbmQtY2VvLXNheXMtYWktYm9vc3RpbmctcHJvZHVjdGl2aXR5LXZpZGVv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiO2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9jZW50cmFsLXByb2Nlc3NpbmctdW5pdC11c2UtY2FzZXMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Seven top central processing unit (CPU) use cases</t>
+          <t>Where Will DevOps Go if IBM Doesn't Make Terraform Open Source Again?</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1551,14 +1551,14 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiO2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9jZW50cmFsLXByb2Nlc3NpbmctdW5pdC11c2UtY2FzZXMv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LndlYnByb25ld3MuY29tL3RlcnJhZm9ybS1vcGVuLXNvdXJjZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>IBM-Spinoff Kyndryl, Apollo Eyeing DXC Technology In Potential Joint Acquisition: Report - Apollo Global Management ...</t>
+          <t>Obituary: Theodor “Ted” Bogner, 1935-2024 | Obituaries</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1568,14 +1568,14 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5iZW56aW5nYS5jb20vbWFya2V0cy9lcXVpdGllcy8yNC8wNi8zOTI2MjYyMy9pYm0tc3Bpbm9mZi1reW5kcnlsLWFwb2xsby1leWVpbmctZHhjLXRlY2hub2xvZ3ktaW4tcG90ZW50aWFsLWpvaW50LWFjcXVpc2l0aW9uLXJlcG9ydNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LnNldmVuZGF5c3Z0LmNvbS9saWZlLWxpbmVzL29iaXR1YXJ5LXRoZW9kb3ItdGVkLWJvZ25lci0xOTM1LTIwMjQtNDEwNzE3MTfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>IBM wins reversal of $1.6 billion judgment to BMC over software contract</t>
+          <t>IBM Inks Deal With Samsung to Build its Latest Chip Processor</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1585,14 +1585,14 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiPmh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vaWJtLXdpbnMtcmV2ZXJzYWwtMS02LTIxMTk1MDg1Ni5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vZmluYW5jZS9uZXdzL2libS1pbmtzLWRlYWwtc2Ftc3VuZy1idWlsZC0xNTMzMDMyODEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>IBM UK &amp; Ireland CEO Nicola Hodson on the AI revolution in business - How to be a CEO podcast</t>
+          <t>IBM UK and Ireland CEO Says AI Boosting Productivity</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1602,14 +1602,14 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQWh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLWNlby1uaWNvbGEtaG9kc29uLWFpLTA4MDAzNjY3MS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy92aWRlb3MvMjAyNC0wNi0xMC9pYm0tdWstYW5kLWlyZWxhbmQtY2VvLXNheXMtYWktYm9vc3RpbmctcHJvZHVjdGl2aXR5LXZpZGVv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>IBM, Cleveland Clinic Team for AI, Quantum in Life Sciences</t>
+          <t>IBM wins reversal of $1.6 billion judgment to BMC over software contract</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1619,14 +1619,14 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vaWJtLWNsZXZlbGFuZC1jbGluaWMtdGVhbS1mb3ItYWktcXVhbnR1bS1pbi1saWZlLXNjaWVuY2Vz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiPmh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vaWJtLXdpbnMtcmV2ZXJzYWwtMS02LTIxMTk1MDg1Ni5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>IBM Inks Deal With Samsung to Build its Latest Chip Processor</t>
+          <t>IBM-Spinoff Kyndryl, Apollo Eyeing DXC Technology In Potential Joint Acquisition: Report - Apollo Global Management ...</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1636,14 +1636,14 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUWh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vZmluYW5jZS9uZXdzL2libS1pbmtzLWRlYWwtc2Ftc3VuZy1idWlsZC0xNTMzMDMyODEuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5iZW56aW5nYS5jb20vbWFya2V0cy9lcXVpdGllcy8yNC8wNi8zOTI2MjYyMy9pYm0tc3Bpbm9mZi1reW5kcnlsLWFwb2xsby1leWVpbmctZHhjLXRlY2hub2xvZ3ktaW4tcG90ZW50aWFsLWpvaW50LWFjcXVpc2l0aW9uLXJlcG9ydNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Where Will DevOps Go if IBM Doesn't Make Terraform Open Source Again?</t>
+          <t>IBM, Cleveland Clinic Team for AI, Quantum in Life Sciences</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1653,65 +1653,65 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMWh0dHBzOi8vd3d3LndlYnByb25ld3MuY29tL3RlcnJhZm9ybS1vcGVuLXNvdXJjZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiX2h0dHBzOi8vd3d3LmlvdHdvcmxkdG9kYXkuY29tL3F1YW50dW0vaWJtLWNsZXZlbGFuZC1jbGluaWMtdGVhbS1mb3ItYWktcXVhbnR1bS1pbi1saWZlLXNjaWVuY2Vz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Obituary: Theodor “Ted” Bogner, 1935-2024 | Obituaries</t>
+          <t>Mosley Wealth Management Buys New Holdings in International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>2024-06-10 18:13:16.600323</t>
+          <t>2024-06-10 18:13:16.607946</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiVWh0dHBzOi8vd3d3LnNldmVuZGF5c3Z0LmNvbS9saWZlLWxpbmVzL29iaXR1YXJ5LXRoZW9kb3ItdGVkLWJvZ25lci0xOTM1LTIwMjQtNDEwNzE3MTfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTAvbW9zbGV5LXdlYWx0aC1tYW5hZ2VtZW50LWJ1eXMtbmV3LWhvbGRpbmdzLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Mosley Wealth Management Buys New Holdings in International Business Machines Co. (NYSE:IBM)</t>
+          <t>IBM and AI Singapore ink collaboration for the 1st LLM developed for SEA</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>2024-06-10 18:13:16.607946</t>
+          <t>2024-06-10 18:13:16.609062</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTAvbW9zbGV5LXdlYWx0aC1tYW5hZ2VtZW50LWJ1eXMtbmV3LWhvbGRpbmdzLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vZnV0dXJlY2lvLnRlY2gvaWJtLWFuZC1haS1zaW5nYXBvcmUtaW5rLWNvbGxhYm9yYXRpb24tZm9yLXRoZS0xc3QtbGxtLWRldmVsb3BlZC1mb3Itc2VhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>IBM and AI Singapore ink collaboration for the 1st LLM developed for SEA</t>
+          <t>IBM (IBM) Stock Drops Despite Market Gains: Important Facts to Note</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>2024-06-10 18:13:16.609062</t>
+          <t>2024-06-11 18:13:16.593704</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYGh0dHBzOi8vZnV0dXJlY2lvLnRlY2gvaWJtLWFuZC1haS1zaW5nYXBvcmUtaW5rLWNvbGxhYm9yYXRpb24tZm9yLXRoZS0xc3QtbGxtLWRldmVsb3BlZC1mb3Itc2VhL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vY2EuZmluYW5jZS55YWhvby5jb20vbmV3cy9pYm0taWJtLXN0b2NrLWRyb3BzLWRlc3BpdGUtMjE0NTE4MDI1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Converge Technology Solutions Announces Contact Center IQ Built on IBM watsonx</t>
+          <t>Leading Banking Technology Firms: Finastra, IBM, Sopra in 2024</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -1721,14 +1721,14 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy5wcm5ld3N3aXJlLmNvbS9uZXdzLXJlbGVhc2VzL2NvbnZlcmdlLXRlY2hub2xvZ3ktc29sdXRpb25zLWFubm91bmNlcy1jb250YWN0LWNlbnRlci1pcS1idWlsdC1vbi1pYm0td2F0c29ueC0zMDIxNjkxNjAuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vZmludGVjaG1hZ2F6aW5lLmNvbS9hcnRpY2xlcy90aGUtbGVhZGluZy1iYW5raW5nLXRlY2hub2xvZ3ktZmlybXMtaW4tMjAyNNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>ContextQA Turns to IBM for AI to Automate Testing</t>
+          <t>IBM Consulting brings hybrid cloud solutions for business growth</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -1738,14 +1738,14 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRWh0dHBzOi8vZGV2b3BzLmNvbS9jb250ZXh0cWEtdHVybnMtdG8taWJtLWZvci1haS10by1hdXRvbWF0ZS10ZXN0aW5nL9IBSWh0dHBzOi8vZGV2b3BzLmNvbS9jb250ZXh0cWEtdHVybnMtdG8taWJtLWZvci1haS10by1hdXRvbWF0ZS10ZXN0aW5nL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vc2lsaWNvbmFuZ2xlLmNvbS8yMDI0LzA2LzExL2libS1jb25zdWx0aW5nLWJyaW5ncy1oeWJyaWQtY2xvdWQtc29sdXRpb25zLWJ1c2luZXNzLWdyb3d0aC1yaHN1bW1pdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Converge Technology unveils Contact Centre IQ built on IBM tech</t>
+          <t>ContextQA Turns to IBM for AI to Automate Testing</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -1755,14 +1755,14 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vc3RvY2tob3VzZS5jb20vbmV3cy90aGUtbWFya2V0LW9ubGluZS1uZXdzLzIwMjQvMDYvMTEvY29udmVyZ2UtdGVjaG5vbG9neS11bnZlaWxzLWNvbnRhY3QtY2VudHJlLWlxLWJ1aWx0LW9uLWlibS10ZWNo0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRWh0dHBzOi8vZGV2b3BzLmNvbS9jb250ZXh0cWEtdHVybnMtdG8taWJtLWZvci1haS10by1hdXRvbWF0ZS10ZXN0aW5nL9IBSWh0dHBzOi8vZGV2b3BzLmNvbS9jb250ZXh0cWEtdHVybnMtdG8taWJtLWZvci1haS10by1hdXRvbWF0ZS10ZXN0aW5nL2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>IBM Consulting brings hybrid cloud solutions for business growth</t>
+          <t>Converge Technology Solutions Announces Contact Center IQ Built on IBM watsonx</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -1772,14 +1772,14 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vc2lsaWNvbmFuZ2xlLmNvbS8yMDI0LzA2LzExL2libS1jb25zdWx0aW5nLWJyaW5ncy1oeWJyaWQtY2xvdWQtc29sdXRpb25zLWJ1c2luZXNzLWdyb3d0aC1yaHN1bW1pdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy5wcm5ld3N3aXJlLmNvbS9uZXdzLXJlbGVhc2VzL2NvbnZlcmdlLXRlY2hub2xvZ3ktc29sdXRpb25zLWFubm91bmNlcy1jb250YWN0LWNlbnRlci1pcS1idWlsdC1vbi1pYm0td2F0c29ueC0zMDIxNjkxNjAuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>IBM dream to gobble up HashiCorp challenged in court</t>
+          <t>Converge Technology unveils Contact Centre IQ built on IBM tech</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -1789,65 +1789,65 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiPWh0dHBzOi8vd3d3LnRoZXJlZ2lzdGVyLmNvbS8yMDI0LzA2LzExL2libV9oYXNoaWNvcnBfbGF3c3VpdC_SAUFodHRwczovL3d3dy50aGVyZWdpc3Rlci5jb20vQU1QLzIwMjQvMDYvMTEvaWJtX2hhc2hpY29ycF9sYXdzdWl0Lw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vc3RvY2tob3VzZS5jb20vbmV3cy90aGUtbWFya2V0LW9ubGluZS1uZXdzLzIwMjQvMDYvMTEvY29udmVyZ2UtdGVjaG5vbG9neS11bnZlaWxzLWNvbnRhY3QtY2VudHJlLWlxLWJ1aWx0LW9uLWlibS10ZWNo0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Leading Banking Technology Firms: Finastra, IBM, Sopra in 2024</t>
+          <t>IBM's Qiskit 1.0 Blazes the Trail</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.593704</t>
+          <t>2024-06-11 18:13:16.598820</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUWh0dHBzOi8vZmludGVjaG1hZ2F6aW5lLmNvbS9hcnRpY2xlcy90aGUtbGVhZGluZy1iYW5raW5nLXRlY2hub2xvZ3ktZmlybXMtaW4tMjAyNNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTEvaWJtcy1xaXNraXQtMS0wLWJsYXplcy10aGUtdHJhaWwv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>IBM (IBM) Stock Drops Despite Market Gains: Important Facts to Note</t>
+          <t>3 Ultra-Cheap Cloud Stocks Worth Watching in June</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.593704</t>
+          <t>2024-06-11 18:13:16.600323</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vY2EuZmluYW5jZS55YWhvby5jb20vbmV3cy9pYm0taWJtLXN0b2NrLWRyb3BzLWRlc3BpdGUtMjE0NTE4MDI1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzLzMtdWx0cmEtY2hlYXAtY2xvdWQtc3RvY2tzLXdvcnRoLXdhdGNoaW5nLWluLWp1bmUtMTAzMzQ2ODM0NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>IBM's Qiskit 1.0 Blazes the Trail</t>
+          <t>4 popular machine learning certificates to get in 2024</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.598820</t>
+          <t>2024-06-11 18:13:16.600323</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTEvaWJtcy1xaXNraXQtMS0wLWJsYXplcy10aGUtdHJhaWwv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LnRlY2h0YXJnZXQuY29tL3NlYXJjaGNsb3VkY29tcHV0aW5nL3RpcC8zLXBvcHVsYXItbWFjaGluZS1sZWFybmluZy1jZXJ0aWZpY2F0aW9ucy10by1nZXQtaW4tMjAyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>4 popular machine learning certificates to get in 2024</t>
+          <t>IBM (IBM) Stock Sinks As Market Gains: What You Should Know</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -1857,14 +1857,14 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vd3d3LnRlY2h0YXJnZXQuY29tL3NlYXJjaGNsb3VkY29tcHV0aW5nL3RpcC8zLXBvcHVsYXItbWFjaGluZS1sZWFybmluZy1jZXJ0aWZpY2F0aW9ucy10by1nZXQtaW4tMjAyMtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUWh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL2ZpbmFuY2UvbmV3cy9pYm0taWJtLXN0b2NrLXNpbmtzLW1hcmtldC0yMTQ1MDk0MjAuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>IBM (IBM) Stock Sinks As Market Gains: What You Should Know</t>
+          <t>As NVIDIA, IBM and others apply AI to boost utilities, regulatory and data privacy obstacles abound</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -1874,14 +1874,14 @@
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUWh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL2ZpbmFuY2UvbmV3cy9pYm0taWJtLXN0b2NrLXNpbmtzLW1hcmtldC0yMTQ1MDk0MjAuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9udmlkaWEtaWJtLW90aGVycy1hcHBseS1haS0wOTAwMDAxMzIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>As NVIDIA, IBM and others apply AI to boost utilities, regulatory and data privacy obstacles abound</t>
+          <t>International Business Machines (NYSE:IBM) Stock Price Down 1.4%</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -1891,150 +1891,150 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSGh0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9udmlkaWEtaWJtLW90aGVycy1hcHBseS1haS0wOTAwMDAxMzIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXBlcmNlbnQtZGVjbGluZS0yMDI0LTA2LTExL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>3 Ultra-Cheap Cloud Stocks Worth Watching in June</t>
+          <t>NatWest prepares to introduce GenAI-powered virtual assistant Cora+ in collaboration with IBM</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.600323</t>
+          <t>2024-06-11 18:13:16.607946</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibGh0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzLzMtdWx0cmEtY2hlYXAtY2xvdWQtc3RvY2tzLXdvcnRoLXdhdGNoaW5nLWluLWp1bmUtMTAzMzQ2ODM0NdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy5maW50ZWNoZnV0dXJlcy5jb20vMjAyNC8wNi9uYXR3ZXN0LXByZXBhcmVzLXRvLWludHJvZHVjZS1nZW5haS1wb3dlcmVkLXZpcnR1YWwtYXNzaXN0YW50LWNvcmEtaW4tY29sbGFib3JhdGlvbi13aXRoLWlibS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>International Business Machines (NYSE:IBM) Stock Price Down 1.4%</t>
+          <t>Containing Damage and Accelerating Recovery from Data Breaches</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.600323</t>
+          <t>2024-06-11 18:13:16.609062</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXBlcmNlbnQtZGVjbGluZS0yMDI0LTA2LTExL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LmZpZXJjZWhlYWx0aGNhcmUuY29tL3ByZW1pdW0vd2ViaW5hci9jb250YWluaW5nLWRhbWFnZS1hbmQtYWNjZWxlcmF0aW5nLXJlY292ZXJ5LWRhdGEtYnJlYWNoZXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>NatWest prepares to introduce GenAI-powered virtual assistant Cora+ in collaboration with IBM</t>
+          <t>21CS Releases Enhanced Version of IBM Streams</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.607946</t>
+          <t>2024-06-12 18:13:16.593704</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy5maW50ZWNoZnV0dXJlcy5jb20vMjAyNC8wNi9uYXR3ZXN0LXByZXBhcmVzLXRvLWludHJvZHVjZS1nZW5haS1wb3dlcmVkLXZpcnR1YWwtYXNzaXN0YW50LWNvcmEtaW4tY29sbGFib3JhdGlvbi13aXRoLWlibS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmFjY2Vzc3dpcmUuY29tLzg3NTk0MC8yMWNzLXJlbGVhc2VzLWVuaGFuY2VkLXZlcnNpb24tb2YtaWJtLXN0cmVhbXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Tech Tuesdays: StockX Battles Counterfeits + IBM on Gen AI Use</t>
+          <t>Bank CEOs want AI ASAP, but workplace resistance persists: IBM survey</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.609062</t>
+          <t>2024-06-12 18:13:16.593704</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbW9uZXkvb3RoZXIvdGVjaC10dWVzZGF5cy1zdG9ja3gtYmF0dGxlcy1jb3VudGVyZmVpdHMtaWJtLW9uLWdlbi1haS11c2UvYXItQkIxbzFtYm7SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vZnAtd29yay9iYW5rLWNlb3MtYWktd29ya3BsYWNlLXJlc2lzdGFuY2UtaWJt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Containing Damage and Accelerating Recovery from Data Breaches</t>
+          <t>IBM-Hashicorp: Shareholder lawsuit seeks to derail $6.4 billion acquisition</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>2024-06-11 18:13:16.609062</t>
+          <t>2024-06-12 18:13:16.593704</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiamh0dHBzOi8vd3d3LmZpZXJjZWhlYWx0aGNhcmUuY29tL3ByZW1pdW0vd2ViaW5hci9jb250YWluaW5nLWRhbWFnZS1hbmQtYWNjZWxlcmF0aW5nLXJlY292ZXJ5LWRhdGEtYnJlYWNoZXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmNpby5jb20vYXJ0aWNsZS8yMTQ0MDI4L2libS1oYXNoaWNvcnAtc2hhcmVob2xkZXItbGF3c3VpdC1zZWVrcy10by1kZXJhaWwtNi00LWJpbGxpb24tYWNxdWlzaXRpb24uaHRtbNIBcmh0dHBzOi8vd3d3LmNpby5jb20vYXJ0aWNsZS8yMTQ0MDI4L2libS1oYXNoaWNvcnAtc2hhcmVob2xkZXItbGF3c3VpdC1zZWVrcy10by1kZXJhaWwtNi00LWJpbGxpb24tYWNxdWlzaXRpb24uaHRtbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>21CS Releases Enhanced Version of IBM Streams</t>
+          <t>Rapidus and IBM Expand Collaboration to Chiplet Packaging Technology</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.593704</t>
+          <t>2024-06-12 18:13:16.600323</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3LmFjY2Vzc3dpcmUuY29tLzg3NTk0MC8yMWNzLXJlbGVhc2VzLWVuaGFuY2VkLXZlcnNpb24tb2YtaWJtLXN0cmVhbXPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmVldGFzaWEuY29tL3JhcGlkdXMtYW5kLWlibS1leHBhbmQtY29sbGFib3JhdGlvbi10by1jaGlwbGV0LXBhY2thZ2luZy10ZWNobm9sb2d5L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Bank CEOs want AI ASAP, but workplace resistance persists: IBM survey</t>
+          <t>GlobalFoundries sues IBM, says trade secrets were unlawfully given to Japan's Rapidus</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.593704</t>
+          <t>2024-06-12 18:13:16.600323</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiR2h0dHBzOi8vZmluYW5jaWFscG9zdC5jb20vZnAtd29yay9iYW5rLWNlb3MtYWktd29ya3BsYWNlLXJlc2lzdGFuY2UtaWJt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTGh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vZ2xvYmFsZm91bmRyaWVzLXN1ZXMtaWJtLXNheXMtdHJhZGUtMTMzODU1MzM2Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>IBM-Hashicorp: Shareholder lawsuit seeks to derail $6.4 billion acquisition</t>
+          <t>International Business Machines (NYSE:IBM) Stock Price Up 0.5%</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.593704</t>
+          <t>2024-06-12 18:13:16.600323</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LmNpby5jb20vYXJ0aWNsZS8yMTQ0MDI4L2libS1oYXNoaWNvcnAtc2hhcmVob2xkZXItbGF3c3VpdC1zZWVrcy10by1kZXJhaWwtNi00LWJpbGxpb24tYWNxdWlzaXRpb24uaHRtbNIBcmh0dHBzOi8vd3d3LmNpby5jb20vYXJ0aWNsZS8yMTQ0MDI4L2libS1oYXNoaWNvcnAtc2hhcmVob2xkZXItbGF3c3VpdC1zZWVrcy10by1kZXJhaWwtNi00LWJpbGxpb24tYWNxdWlzaXRpb24uaHRtbA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXBlcmNlbnQtYWR2YW5jZS0yMDI0LTA2LTEyL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Rapidus and IBM Expand Collaboration to Chiplet Packaging Technology</t>
+          <t>Generative AI Could Significantly Improve Product Innovation, Says IBM | ESM Magazine</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2044,14 +2044,14 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmVldGFzaWEuY29tL3JhcGlkdXMtYW5kLWlibS1leHBhbmQtY29sbGFib3JhdGlvbi10by1jaGlwbGV0LXBhY2thZ2luZy10ZWNobm9sb2d5L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LmVzbW1hZ2F6aW5lLmNvbS90ZWNobm9sb2d5L2dlbmVyYXRpdmUtYWktY291bGQtc2lnbmlmaWNhbnRseS1pbXByb3ZlLXByb2R1Y3QtaW5ub3ZhdGlvbi1zYXlzLWlibS0yNjcyMDTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>GlobalFoundries sues IBM, says trade secrets were unlawfully given to Japan's Rapidus</t>
+          <t>IBM on Transformation to AI-Enabled Experiences</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2061,75 +2061,75 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTGh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vZ2xvYmFsZm91bmRyaWVzLXN1ZXMtaWJtLXNheXMtdHJhZGUtMTMzODU1MzM2Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy92aWRlb3MvMjAyNC0wNi0xMi9pYm0tb24tdHJhbnNmb3JtYXRpb24tdG8tYWktZW5hYmxlZC1leHBlcmllbmNlcy12aWRlb9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>International Business Machines (NYSE:IBM) Stock Price Up 0.5%</t>
+          <t>Adobe Employees Slam the Company Over AI Controversy</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.600323</t>
+          <t>2024-06-12 18:13:16.607946</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXBlcmNlbnQtYWR2YW5jZS0yMDI0LTA2LTEyL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmJ1c2luZXNzaW5zaWRlci5jb20vYWRvYmUtZW1wbG95ZWVzLXNsYW0tY29tcGFueS1vdmVyLWFpLWNvbnRyb3ZlcnN5LTIwMjQtNtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Generative AI Could Significantly Improve Product Innovation, Says IBM | ESM Magazine</t>
+          <t>CIO Streamlines Corporate Data Governance</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vd3d3LmVzbW1hZ2F6aW5lLmNvbS90ZWNobm9sb2d5L2dlbmVyYXRpdmUtYWktY291bGQtc2lnbmlmaWNhbnRseS1pbXByb3ZlLXByb2R1Y3QtaW5ub3ZhdGlvbi1zYXlzLWlibS0yNjcyMDTSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLmh0dHBzOi8vd3d3LmlibS5jb20vY2FzZS1zdHVkaWVzL29wZW5wYWdlcy1ncmPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>IBM on Transformation to AI-Enabled Experiences</t>
+          <t>IBM Bets Big on $1T Hybrid Cloud Market With Business Spin-off</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmJsb29tYmVyZy5jb20vbmV3cy92aWRlb3MvMjAyNC0wNi0xMi9pYm0tb24tdHJhbnNmb3JtYXRpb24tdG8tYWktZW5hYmxlZC1leHBlcmllbmNlcy12aWRlb9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL3N0eWxlL2libS1iZXRzLWJpZy0xdC1oeWJyaWQtMTMzNDAxNzc1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Adobe Employees Slam the Company Over AI Controversy</t>
+          <t>IBM thinks it's ready to turn quantum computing into an actual business</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>2024-06-12 18:13:16.607946</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmJ1c2luZXNzaW5zaWRlci5jb20vYWRvYmUtZW1wbG95ZWVzLXNsYW0tY29tcGFueS1vdmVyLWFpLWNvbnRyb3ZlcnN5LTIwMjQtNtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLXRoaW5rcy1yZWFkeS10dXJuLXF1YW50dW0tMDUwMTAwNTc0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.593704</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
@@ -2153,68 +2153,68 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Best practices for augmenting human intelligence with AI</t>
+          <t>The time is now for quantum-readiness</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.593704</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9iZXN0LXByYWN0aWNlcy1mb3ItYXVnbWVudGluZy1odW1hbi1pbnRlbGxpZ2VuY2Utd2l0aC1haS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiPWh0dHBzOi8vZnV0dXJlY2lvLnRlY2gvdGhlLXRpbWUtaXMtbm93LWZvci1xdWFudHVtLXJlYWRpbmVzcy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>boxxe</t>
+          <t>Far East Organization</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.598820</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiJmh0dHBzOi8vd3d3LmlibS5jb20vY2FzZS1zdHVkaWVzL2JveHhl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiNmh0dHBzOi8vd3d3LmlibS5jb20vY2FzZS1zdHVkaWVzL2Zhci1lYXN0LW9yZ2FuaXphdGlvbtIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Cannes Lions 2024</t>
+          <t>Transcript: The Futurist Summit: The Age of AI: The Future of AI is Open: Sponsored by IBM</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.598820</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiIWh0dHBzOi8vd3d3LmlibS5jb20vZXZlbnRzL2Nhbm5lc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy53YXNoaW5ndG9ucG9zdC5jb20vd2FzaGluZ3Rvbi1wb3N0LWxpdmUvMjAyNC8wNi8xMy90cmFuc2NyaXB0LWZ1dHVyaXN0LXN1bW1pdC1hZ2UtYWktZnV0dXJlLWFpLWlzLW9wZW4tc3BvbnNvcmVkLWJ5LWlibS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>AMD CEO Lisa Su reminisces about designing the PS3's infamous Cell processor during her time at IBM</t>
+          <t>boxxe</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMif2h0dHBzOi8vd3d3LnRvbXNoYXJkd2FyZS5jb20vdGVjaC1pbmR1c3RyeS9hbWQtY2VvLWxpc2Etc3UtcmVtaW5pc2Nlcy1vbi1oZWxwaW5nLWRlc2lnbi10aGUtcHMzcy1pbmZhbW91cy1jZWxsLXByb2Nlc3Nvci1hdC1pYm3SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiJmh0dHBzOi8vd3d3LmlibS5jb20vY2FzZS1zdHVkaWVzL2JveHhl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
@@ -2226,7 +2226,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -2238,1037 +2238,2431 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>IBM to invest $1 billion to create new business unit for Watson</t>
+          <t>WPP</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRGh0dHBzOi8vYXUubmV3cy55YWhvby5jb20vaWJtLWludmVzdC0xLWJpbGxpb24tY3JlYXRlLTA3MTU0NzY5MC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiJGh0dHBzOi8vd3d3LmlibS5jb20vY2FzZS1zdHVkaWVzL3dwcNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>IBM Bets Big on $1T Hybrid Cloud Market With Business Spin-off</t>
+          <t>Best practices for augmenting human intelligence with AI</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vdWsuc3R5bGUueWFob28uY29tL3N0eWxlL2libS1iZXRzLWJpZy0xdC1oeWJyaWQtMTMzNDAxNzc1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9iZXN0LXByYWN0aWNlcy1mb3ItYXVnbWVudGluZy1odW1hbi1pbnRlbGxpZ2VuY2Utd2l0aC1haS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>IBM thinks it's ready to turn quantum computing into an actual business</t>
+          <t>IBM to invest $1 billion to create new business unit for Watson</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.707990</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vbnoubmV3cy55YWhvby5jb20vaWJtLXRoaW5rcy1yZWFkeS10dXJuLXF1YW50dW0tMDUwMTAwNTc0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRGh0dHBzOi8vYXUubmV3cy55YWhvby5jb20vaWJtLWludmVzdC0xLWJpbGxpb24tY3JlYXRlLTA3MTU0NzY5MC5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>What Is the Levelized Cost of Energy (LCOE)?</t>
+          <t>U.S.-Japan Foundry Cooperation Intensifies: A Threat to Samsung Electronics?</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiOWh0dHBzOi8vd3d3LmlibS5jb20vdGhpbmsvdG9waWNzL2xldmVsaXplZC1jb3N0LW9mLWVuZXJnedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiQmh0dHBzOi8vd3d3LmJ1c2luZXNza29yZWEuY28ua3IvbmV3cy9hcnRpY2xlVmlldy5odG1sP2lkeG5vPTIxOTA1NNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>What is an AI accelerator?</t>
+          <t>Kerala to host international Gen AI conclave in partnership with IBM</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiL2h0dHBzOi8vd3d3LmlibS5jb20vdGhpbmsvdG9waWNzL2FpLWFjY2VsZXJhdG9y0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiggFodHRwczovL2VuZ2xpc2gubWF0aHJ1Ymh1bWkuY29tL2ZlYXR1cmVzL3RlY2hub2xvZ3kva2VyYWxhLXRvLWhvc3QtaW50ZXJuYXRpb25hbC1nZW4tYWktY29uY2xhdmUtaW4tcGFydG5lcnNoaXAtd2l0aC1pYm0tMS45NjM1NTE50gGGAWh0dHBzOi8vZW5nbGlzaC5tYXRocnViaHVtaS5jb20vYW1wL2ZlYXR1cmVzL3RlY2hub2xvZ3kva2VyYWxhLXRvLWhvc3QtaW50ZXJuYXRpb25hbC1nZW4tYWktY29uY2xhdmUtaW4tcGFydG5lcnNoaXAtd2l0aC1pYm0tMS45NjM1NTE5?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Transcript: The Futurist Summit: The Age of AI: The Future of AI is Open: Sponsored by IBM</t>
+          <t>Kerala partners with IBM to host global conclave on Gen AI</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihAFodHRwczovL3d3dy53YXNoaW5ndG9ucG9zdC5jb20vd2FzaGluZ3Rvbi1wb3N0LWxpdmUvMjAyNC8wNi8xMy90cmFuc2NyaXB0LWZ1dHVyaXN0LXN1bW1pdC1hZ2UtYWktZnV0dXJlLWFpLWlzLW9wZW4tc3BvbnNvcmVkLWJ5LWlibS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicmh0dHBzOi8vaW4uaW52ZXN0aW5nLmNvbS9uZXdzL3N0b2NrLW1hcmtldC1uZXdzL2tlcmFsYS1wYXJ0bmVycy13aXRoLWlibS10by1ob3N0LWdsb2JhbC1jb25jbGF2ZS1vbi1nZW4tYWktNDI1MTU4MNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Kerala partners with IBM to host global conclave on Gen AI</t>
+          <t>Sevilla FC uses AI-Powered Scout Advisor from IBM for player recruitment</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>2024-06-13 18:13:16.607946</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vaW5kaWFuZXdlbmdsYW5kLmNvbS9rZXJhbGEtcGFydG5lcnMtd2l0aC1pYm0tdG8taG9zdC1nbG9iYWwtY29uY2xhdmUtb24tZ2VuLWFpL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMif2h0dHBzOi8vaW5mb3RlY2hsZWFkLmNvbS9hcnRpZmljaWFsLWludGVsbGlnZW5jZS9zZXZpbGxhLWZjLXVzZXMtYWktcG93ZXJlZC1zY291dC1hZHZpc29yLWZyb20taWJtLWZvci1wbGF5ZXItcmVjcnVpdG1lbnQtODUzMjfSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>McDonald's is ending its drive-thru AI test</t>
+          <t>Kerala government partners with IBM to host global conclave on Gen AI</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.593704</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vcmVzdGF1cmFudGJ1c2luZXNzb25saW5lLmNvbS90ZWNobm9sb2d5L21jZG9uYWxkcy1lbmRpbmctaXRzLWRyaXZlLXRocnUtYWktdGVzdNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidGh0dHBzOi8vd3d3Lm5ld3M5bGl2ZS5jb20vc3RhdGUva2VyYWxhL2tlcmFsYS1nb3Zlcm5tZW50LXBhcnRuZXJzLXdpdGgtaWJtLXRvLWhvc3QtZ2xvYmFsLWNvbmNsYXZlLW9uLWdlbi1haS0yNTc1OTQ10gF4aHR0cHM6Ly93d3cubmV3czlsaXZlLmNvbS9zdGF0ZS9rZXJhbGEva2VyYWxhLWdvdmVybm1lbnQtcGFydG5lcnMtd2l0aC1pYm0tdG8taG9zdC1nbG9iYWwtY29uY2xhdmUtb24tZ2VuLWFpLTI1NzU5NDUvYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>How Classical AI is 'Saving' Quantum Computing: A Talk with IBM's Ismael Faro</t>
+          <t>Kerala Partners with IBM to Host Global Conclave on Generative AI</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.593704</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigQFodHRwczovL3d3dy5zaWxpY29uaW5kaWEuY29tL25ld3MvZ2VuZXJhbC9rZXJhbGEtcGFydG5lcnMtd2l0aC1pYm0tdG8taG9zdC1nbG9iYWwtY29uY2xhdmUtb24tZ2VuZXJhdGl2ZS1haS1uaWQtMjMwMTY3LWNpZC0xLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Making HTTPS redirects easy with IBM NS1 Connect</t>
+          <t>T-Mobile unlocks marketing efficiency with Adobe Workfront</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.598707</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvbWFraW5nLWh0dHBzLXJlZGlyZWN0cy1lYXN5LXdpdGgtaWJtLW5zMS1jb25uZWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vd3d3LmlibS5jb20vYmxvZy90LW1vYmlsZS11bmxvY2tzLW1hcmtldGluZy1lZmZpY2llbmN5LXdpdGgtYWRvYmUtd29ya2Zyb250L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Lynn Conway, microchip pioneer who overcame transgender discrimination, dies at 86</t>
+          <t>IBM Resets Antitrust Review Clock For $6.4B HashiCorp Buy</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.598820</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8va2l0Y2hlbmVyLmNpdHluZXdzLmNhLzIwMjQvMDYvMTQvbHlubi1jb253YXktbWljcm9jaGlwLXBpb25lZXItd2hvLW92ZXJjYW1lLXRyYW5zZ2VuZGVyLWRpc2NyaW1pbmF0aW9uLWRpZXMtYXQtODYv0gF-aHR0cHM6Ly9raXRjaGVuZXIuY2l0eW5ld3MuY2EvMjAyNC8wNi8xNC9seW5uLWNvbndheS1taWNyb2NoaXAtcGlvbmVlci13aG8tb3ZlcmNhbWUtdHJhbnNnZW5kZXItZGlzY3JpbWluYXRpb24tZGllcy1hdC04Ni9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiYGh0dHBzOi8vd3d3LmxhdzM2MC5jb20vYXJ0aWNsZXMvMTg0NzU0NC9pYm0tcmVzZXRzLWFudGl0cnVzdC1yZXZpZXctY2xvY2stZm9yLTYtNGItaGFzaGljb3JwLWJ1edIBK2h0dHBzOi8vd3d3LmxhdzM2MC5jb20vYW1wL2FydGljbGVzLzE4NDc1NDQ?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>IBM and SAP Gen AI Solutions Elevate Business Excellence</t>
+          <t>AMD CEO Lisa Su reminisces about designing the PS3's…</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.598820</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vaW5zaWRlc2FwLmNvbS9pYm0tYW5kLXNhcC1nZW4tYWktc29sdXRpb25zLWVsZXZhdGUtYnVzaW5lc3MtZXhjZWxsZW5jZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3Lmlua2wuY29tL25ld3MvYW1kLWNlby1saXNhLXN1LXJlbWluaXNjZXMtYWJvdXQtZGVzaWduaW5nLXRoZS1wczMtcy1pbmZhbW91cy1jZWxsLXByb2Nlc3Nvci1kdXJpbmctaGVyLXRpbWUtYXQtaWJt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Guest Viewpoint: Former IBM campus shaping up after years of neglect</t>
+          <t>Developer Of Former IBM/HNA Center Presents Revised Plan With Additional Housing Density</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3LnByZXNzY29ubmVjdHMuY29tL3N0b3J5L29waW5pb24vMjAyNC8wNi8xNC9mb3JtZXItZW5kaWNvdHQtaWJtLWNhbXB1cy1kZXZlbG9wbWVudC1waG9lbml4LWludmVzdG9ycy83NDA3NDQxMTAwNy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vcmNiaXpqb3VybmFsLmNvbS8yMDI0LzA2LzEzL2RldmVsb3Blci1vZi1mb3JtZXItaWJtLWhuYS1jZW50ZXItcHJlc2VudHMtcmV2aXNlZC1wbGFuLXdpdGgtYWRkaXRpb25hbC1kZW5zaXR5L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>International Business Machines (NYSE:IBM) Shares Down 0.7%</t>
+          <t>Lynn Conway, microchip pioneer and trans rights advocate, dies at 86</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiTmh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXBlcmNlbnQtZGVjbGluZS0yMDI0LTA2LTE0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vd3d3Lndhc2hpbmd0b25wb3N0LmNvbS9vYml0dWFyaWVzLzIwMjQvMDYvMTMvbHlubi1jb253YXktZGVhZC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>International Business Machines Corporation (IBM) is Attracting Investor Attention: Here is What You Should Know</t>
+          <t>Bayesian Capital Management LP Buys Shares of 39388 International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiuwFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL21vbmV5L21hcmtldHMvaW50ZXJuYXRpb25hbC1idXNpbmVzcy1tYWNoaW5lcy1jb3Jwb3JhdGlvbi1pYm0taXMtYXR0cmFjdGluZy1pbnZlc3Rvci1hdHRlbnRpb24taGVyZS1pcy13aGF0LXlvdS1zaG91bGQta25vdy9hci1CQjFvZWVYTT9vY2lkPWZpbmFuY2UtdmVydGhwLWZlZWRz0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTMvYmF5ZXNpYW4tY2FwaXRhbC1tYW5hZ2VtZW50LWxwLWJ1eXMtc2hhcmVzLW9mLTM5Mzg4LWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>A Closer Look at IBM's Options Market Dynamics - IBM (NYSE:IBM)</t>
+          <t>Former IBM Endicott Site Could Host Residential Project</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMieWh0dHBzOi8vd3d3LmJlbnppbmdhLmNvbS9pbnNpZ2h0cy9vcHRpb25zLzI0LzA2LzM5MzM1MzY5L2EtY2xvc2VyLWxvb2stYXQtaWJtcy1vcHRpb25zLW1hcmtldC1keW5hbWljcz9jb21tZW50c19vcGVuPXRydWXSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiOWh0dHBzOi8vd25iZi5jb20vZm9ybWVyLWlibS1lbmRpY290dC1yZXNpZGVudGlhbC1wcm9qZWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Wealthquest Corp Sells 1641 Shares of International Business Machines Co. (NYSE:IBM)</t>
+          <t>IBM pulls, refiles HSR notification for HashiCorp deal</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.600323</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LmRlZmVuc2V3b3JsZC5uZXQvMjAyNC8wNi8xNC93ZWFsdGhxdWVzdC1jb3JwLXNlbGxzLTE2NDEtc2hhcmVzLW9mLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMia2h0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbW9uZXkvY29tcGFuaWVzL2libS1wdWxscy1yZWZpbGVzLWhzci1ub3RpZmljYXRpb24tZm9yLWhhc2hpY29ycC1kZWFsL2FyLUJCMW85S3M20gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Extra Shot - part 5 featuring Appledore Research, and Pliant.io (IBM)</t>
+          <t>3 OG Cryptos Quietly Lockin' Down the Blockchain Turf</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>2024-06-14 18:13:16.607946</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnRlbGVjb210di5jb20vY29udGVudC9kc3AtbGVhZGVycy1mb3J1bS9leHRyYS1zaG90LXBhcnQtNS1mZWF0dXJpbmctYXBwbGVkb3JlLXJlc2VhcmNoLWFuZC1wbGlhbnQtaW8taWJtLTUwNjE4L9IBf2h0dHBzOi8vd3d3LnRlbGVjb210di5jb20vY29udGVudC9kc3AtbGVhZGVycy1mb3J1bS9leHRyYS1zaG90LXBhcnQtNS1mZWF0dXJpbmctYXBwbGVkb3JlLXJlc2VhcmNoLWFuZC1wbGlhbnQtaW8taWJtLTUwNjE4L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMib2h0dHBzOi8vbWFya2V0cy5idXNpbmVzc2luc2lkZXIuY29tL25ld3Mvc3RvY2tzLzMtb2ctY3J5cHRvcy1xdWlldGx5LWxvY2tpbi1kb3duLXRoZS1ibG9ja2NoYWluLXR1cmYtMTAzMzQ3NTU4ONIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Lynn Conway, Computing Pioneer and Transgender Advocate, Dies at 86</t>
+          <t>Kerala partners with IBM to host global conclave on Gen AI in Kochi</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-13 14:15:06.718936</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3d3Lm55dGltZXMuY29tLzIwMjQvMDYvMTUvdGVjaG5vbG9neS9seW5uLWNvbndheS1kZWFkLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy50aGVoaW5kdS5jb20vbmV3cy9uYXRpb25hbC9rZXJhbGEva2VyYWxhLXBhcnRuZXJzLXdpdGgtaWJtLXRvLWhvc3QtZ2xvYmFsLWNvbmNsYXZlLW9uLWdlbi1haS1pbi1rb2NoaS9hcnRpY2xlNjgyODYyNDIuZWNl0gGKAWh0dHBzOi8vd3d3LnRoZWhpbmR1LmNvbS9uZXdzL25hdGlvbmFsL2tlcmFsYS9rZXJhbGEtcGFydG5lcnMtd2l0aC1pYm0tdG8taG9zdC1nbG9iYWwtY29uY2xhdmUtb24tZ2VuLWFpLWluLWtvY2hpL2FydGljbGU2ODI4NjI0Mi5lY2UvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>Taylor Financial Group Inc. Takes $209000 Position in International Business Machines Co. (NYSE:IBM)</t>
+          <t>IBM's Chet Murphy joins CHTTP team</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTUvdGF5bG9yLWZpbmFuY2lhbC1ncm91cC1pbmMtdGFrZXMtMjA5MDAwLXBvc2l0aW9uLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiWmh0dHBzOi8vYXUubGlmZXN0eWxlLnlhaG9vLmNvbS9saWZlc3R5bGUvMjAwNy0xMS0wOC1pYm1zLWNoZXQtbXVycGh5LWpvaW5zLWNodHRwLXRlYW0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Lynn Conway has passed.</t>
+          <t>IBM and SAP Gen AI Solutions Elevate Business Excellence</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LmRhaWx5a29zLmNvbS9zdG9yaWVzLzIwMjQvNi8xNS8yMjQ2ODQxLy1MeW5uLUNvbndheS1oYXMtcGFzc2Vk0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vaW5zaWRlc2FwLmNvbS9pYm0tYW5kLXNhcC1nZW4tYWktc29sdXRpb25zLWVsZXZhdGUtYnVzaW5lc3MtZXhjZWxsZW5jZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>The Dividend Dukes: 3 Stocks That Will Elevate Your Portfolio's Nobility</t>
+          <t>IBM Workers Lose Appeal Over Arbitrator's Nix of Age Bias Claims</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbW9uZXkvdG9wc3RvY2tzL3RoZS1kaXZpZGVuZC1kdWtlcy0zLXN0b2Nrcy10aGF0LXdpbGwtZWxldmF0ZS15b3VyLXBvcnRmb2xpby1zLW5vYmlsaXR5L2FyLUJCMW9hQWVi0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiaGh0dHBzOi8vbmV3cy5ibG9vbWJlcmdsYXcuY29tL2xpdGlnYXRpb24vaWJtLXdvcmtlcnMtbG9zZS1hcHBlYWwtb3Zlci1hcmJpdHJhdG9ycy1uaXgtb2YtYWdlLWJpYXMtY2xhaW1z0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Top multinational companies bet big on Hyderabad's commercial real estate market, lease 8.7 lakh sq ft of office space</t>
+          <t>Lynn Conway, microchip pioneer who overcame transgender discrimination, dies at 86</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy5tc24uY29tL2VuLWluL25ld3MvSW5kaWEvdG9wLW11bHRpbmF0aW9uYWwtY29tcGFuaWVzLWJldC1iaWctb24taHlkZXJhYmFkLXMtY29tbWVyY2lhbC1yZWFsLWVzdGF0ZS1tYXJrZXQtbGVhc2UtOC03LWxha2gtc3EtZnQtb2Ytb2ZmaWNlLXNwYWNlL2FyLUJCMW8xYjhnP29jaWQ9TEVOREhQ0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8va2l0Y2hlbmVyLmNpdHluZXdzLmNhLzIwMjQvMDYvMTQvbHlubi1jb253YXktbWljcm9jaGlwLXBpb25lZXItd2hvLW92ZXJjYW1lLXRyYW5zZ2VuZGVyLWRpc2NyaW1pbmF0aW9uLWRpZXMtYXQtODYv0gF-aHR0cHM6Ly9raXRjaGVuZXIuY2l0eW5ld3MuY2EvMjAyNC8wNi8xNC9seW5uLWNvbndheS1taWNyb2NoaXAtcGlvbmVlci13aG8tb3ZlcmNhbWUtdHJhbnNnZW5kZXItZGlzY3JpbWluYXRpb24tZGllcy1hdC04Ni9hbXAv?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Red Hat Launches RHEL AI and InstructLab to Bring Generative AI to the Enterprise</t>
+          <t>How Classical AI is 'Saving' Quantum Computing: A Talk with IBM's Ismael Faro</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3Lmdsb2JhbHZpbGxhZ2VzcGFjZS5jb20vdGVjaC9yZWQtaGF0LWxhdW5jaGVzLXJoZWwtYWktYW5kLWluc3RydWN0bGFiLXRvLWJyaW5nLWdlbmVyYXRpdmUtYWktdG8tdGhlLWVudGVycHJpc2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMic2h0dHBzOi8vdGhlcXVhbnR1bWluc2lkZXIuY29tLzIwMjQvMDYvMTQvaG93LWNsYXNzaWNhbC1haS1pcy1zYXZpbmctcXVhbnR1bS1jb21wdXRpbmctYS10YWxrLXdpdGgtaWJtcy1pc21hZWwtZmFyby_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Stock market today: Dow sidesteps tech wreck to keep winning streak alive</t>
+          <t>A Closer Look at IBM's Options Market Dynamics - IBM (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiUGh0dHBzOi8vY2Euc3R5bGUueWFob28uY29tL3N0eWxlL3N0b2NrLW1hcmtldC10b2RheS1kb3ctc2lkZXN0ZXBzLTE2MTcwMzI5Ni5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmJlbnppbmdhLmNvbS9pbnNpZ2h0cy9vcHRpb25zLzI0LzA2LzM5MzM1MzY5L2EtY2xvc2VyLWxvb2stYXQtaWJtcy1vcHRpb25zLW1hcmtldC1keW5hbWljc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>How to make boot media for PowerPC Macs on modern hardware - Mac Software Discussions on AppleInsider Forums</t>
+          <t>Making HTTPS redirects easy with IBM NS1 Connect</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiMWh0dHBzOi8vZm9ydW1zLmFwcGxlaW5zaWRlci5jb20vZGlzY3Vzc2lvbi8yMzY3NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vd3d3LmlibS5jb20vYmxvZy9hbm5vdW5jZW1lbnQvbWFraW5nLWh0dHBzLXJlZGlyZWN0cy1lYXN5LXdpdGgtaWJtLW5zMS1jb25uZWN0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>3 Tech Stocks With A History Of Reliable Dividends</t>
+          <t>Wealthquest Corp Sells 1641 Shares of International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiT2h0dHBzOi8vdWsuZmluYW5jZS55YWhvby5jb20vbmV3cy8zLXRlY2gtc3RvY2tzLWhpc3RvcnktcmVsaWFibGUtMTcxMjM0NzM0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3LmRlZmVuc2V3b3JsZC5uZXQvMjAyNC8wNi8xNC93ZWFsdGhxdWVzdC1jb3JwLXNlbGxzLTE2NDEtc2hhcmVzLW9mLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Abandoned History: Oldsmobile's Guidestar Navigation System and Other Cartography (Part V)</t>
+          <t>Extra Shot - part 5 featuring Appledore Research, and Pliant.io (IBM)</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMitwFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL21vbmV5L2NvbXBhbmllcy9hYmFuZG9uZWQtaGlzdG9yeS1vbGRzbW9iaWxlLXMtZ3VpZGVzdGFyLW5hdmlnYXRpb24tc3lzdGVtLWFuZC1vdGhlci1jYXJ0b2dyYXBoeS1wYXJ0LXYvYXItQUExbHpKSmM_aXRlbT1mbGlnaHRzcHJnLXRpcHN1YnNjLXYxYT9zZWFzb249MjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LnRlbGVjb210di5jb20vY29udGVudC9kc3AtbGVhZGVycy1mb3J1bS9leHRyYS1zaG90LXBhcnQtNS1mZWF0dXJpbmctYXBwbGVkb3JlLXJlc2VhcmNoLWFuZC1wbGlhbnQtaW8taWJtLTUwNjE4L9IBf2h0dHBzOi8vd3d3LnRlbGVjb210di5jb20vY29udGVudC9kc3AtbGVhZGVycy1mb3J1bS9leHRyYS1zaG90LXBhcnQtNS1mZWF0dXJpbmctYXBwbGVkb3JlLXJlc2VhcmNoLWFuZC1wbGlhbnQtaW8taWJtLTUwNjE4L2FtcC8?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Lynn Conway, Microchip Pioneer who Overcame Transgender Discrimination, Dies at 86 | EDGE United States</t>
+          <t>International Business Machines Corporation (IBM) is Attracting Investor Attention: Here is What You Should Know</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.707990</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiLWh0dHBzOi8vd3d3LmVkZ2VtZWRpYW5ldHdvcmsuY29tL3N0b3J5LzMzMzgyOdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vZmluYW5jZS55YWhvby5jb20vbmV3cy9pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvcnBvcmF0aW9uLWlibS0xMzAwMTcxNjIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Raymond G. Guillet</t>
+          <t>13634 Shares in International Business Machines Co. (NYSE:IBM) Bought by Optimist Retirement Group LLC</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.718432</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LnJlcC1hbS5jb20vb2JpdHVhcmllcy8yMDI0LzA2LzE1L3JheW1vbmQtZy1ndWlsbGV0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMijwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTQvMTM2MzQtc2hhcmVzLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS1ib3VnaHQtYnktb3B0aW1pc3QtcmV0aXJlbWVudC1ncm91cC1sbGMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Able Wealth Management LLC Purchases Shares of 419 International Business Machines Co. (NYSE:IBM)</t>
+          <t>IBM dream to gobble up HashiCorp challenged in court</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.718432</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiigFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTUvYWJsZS13ZWFsdGgtbWFuYWdlbWVudC1sbGMtcHVyY2hhc2VzLXNoYXJlcy1vZi00MTktaW50ZXJuYXRpb25hbC1idXNpbmVzcy1tYWNoaW5lcy1jby1ueXNlaWJtLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMikgFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL21vbmV5L21hcmtldHMvaWJtLWRyZWFtLXRvLWdvYmJsZS11cC1oYXNoaWNvcnAtY2hhbGxlbmdlZC1pbi1jb3VydC9hci1CQjFvMkFoUT9pdGVtPWZsaWdodHNwcmctdGlwc3Vic2MtdjFhP3NlYXNvbj0yMDI0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Thomas Stone Obituary (2024) - Savannah, GA - Fox &amp; Weeks Funeral Directors - Hodgson Chapel</t>
+          <t>Public Employees Retirement System of Ohio Purchases 6527 Shares of International Business Machines Co. (NYSE ...</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmxlZ2FjeS5jb20vdXMvb2JpdHVhcmllcy9uYW1lL3Rob21hcy1zdG9uZS1vYml0dWFyeT9pZD01NTM1MzAzNNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMimwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTQvcHVibGljLWVtcGxveWVlcy1yZXRpcmVtZW50LXN5c3RlbS1vZi1vaGlvLXB1cmNoYXNlcy02NTI3LXNoYXJlcy1vZi1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvLW55c2VpYm0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Orangetown Accedes To "Emergency" Request From Developer Who Wants To Build 342 Units At Former IBM/HNA ...</t>
+          <t>Guest Viewpoint: Former IBM campus shaping up after years of neglect</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.889417</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMipAFodHRwczovL3JjYml6am91cm5hbC5jb20vMjAyNC8wNi8xNS9vcmFuZ2V0b3duLWFjY2VkZXMtdG8tZW1lcmdlbmN5LXJlcXVlc3QtZnJvbS1kZXZlbG9wZXItd2hvLXdhbnRzLXRvLWJ1aWxkLTM0Mi11bml0cy1hdC1mb3JtZXItaWJtLWhuYS1wYWxpc2FkZXMtdHJhaW5pbmctY2VudGVyL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiRGh0dHBzOi8vd3d3LmFvbC5jb20vZ3Vlc3Qtdmlld3BvaW50LWZvcm1lci1pYm0tY2FtcHVzLTA5MDUzOTIwMy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>GDPR Services Market Booming Worldwide with Latest Trend and Future scope with Top Key Players- IBM, Veritas ...</t>
+          <t>Nancy Elizabeth Hamilton Obituary</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9nZHByLXNlcnZpY2VzLW1hcmtldC1ib29taW5nLXdvcmxkd2lkZS13aXRoLWxhdGVzdC10cmVuZC1hbmQtZnV0dXJlLXNjb3BlLXdpdGgtdG9wLWtleS1wbGF5ZXJzLWlibS12ZXJpdGFzLWF3cy1taWNyb3NvZnQvNzExNDUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiL2h0dHBzOi8vd3d3Lmtub3huZXdzLmNvbS9vYml0dWFyaWVzL3Bva3IwODUzMjAw0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>IT safety: Linux is weak - expat IT safety alert replace (vulnerability: medium)</t>
+          <t>IBM Cuts Workers' Hours to Save Money</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9pdC1zYWZldHktbGludXgtaXMtd2Vhay1leHBhdC1pdC1zYWZldHktYWxlcnQtcmVwbGFjZS12dWxuZXJhYmlsaXR5LW1lZGl1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSGh0dHBzOi8vd3d3LmFvbC5jb20vMjAxMy0wNS0wMi1pYm0tY3V0cy13b3JrZXJzLWhvdXJzLXRvLXNhdmUtbW9uZXkuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>IT safety: Linux, macOS X and UNIX are threatened - IT safety alert replace for Node.js (danger: medium)</t>
+          <t>Microchip Design Pioneer Lynn Conway Dies at 86, Overcoming Transgender Discrimination</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5icmVha2luZ2xhdGVzdC5uZXdzL3RlY2hub2xvZ3kvaXQtc2FmZXR5LWxpbnV4LW1hY29zLXgtYW5kLXVuaXgtYXJlLXRocmVhdGVuZWQtaXQtc2FmZXR5LWFsZXJ0LXJlcGxhY2UtZm9yLW5vZGUtanMtZGFuZ2VyLW1lZGl1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3RlY2h0aW1lcy5jb20vYXJ0aWNsZXMvMzA1NzE3LzIwMjQwNjE0L21pY3JvY2hpcC1kZXNpZ24tcGlvbmVlci1seW5uLWNvbndheS1kaWVzLTg2LW92ZXJjb21pbmctdHJhbnNnZW5kZXItZGlzY3JpbWluYXRpb24uaHRt0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>Anything-as-a-Service Market will touch a new level in upcoming year with Top Key Players like Cisco, Google, IBM ...</t>
+          <t>An Attempt to Mine Bitcoin on 1960s IBM Mainframe</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMirQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9hbnl0aGluZy1hcy1hLXNlcnZpY2UtbWFya2V0LXdpbGwtdG91Y2gtYS1uZXctbGV2ZWwtaW4tdXBjb21pbmcteWVhci13aXRoLXRvcC1rZXktcGxheWVycy1saWtlLWNpc2NvLWdvb2dsZS1pYm0tbWljcm9zb2Z0LzcxMTQ3L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vd3d3Lm5ld3NidGMuY29tL25ld3MvYW4tYXR0ZW1wdC10by1taW5lLWJpdGNvaW4tb24tMTk2MHMtaWJtLW1haW5mcmFtZS_SAVNodHRwczovL3d3dy5uZXdzYnRjLmNvbS9uZXdzL2FuLWF0dGVtcHQtdG8tbWluZS1iaXRjb2luLW9uLTE5NjBzLWlibS1tYWluZnJhbWUvYW1wLw?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>Sales Performance Management (SPM) Market Breaking New Grounds and Touch New Level in upcoming year by ...</t>
+          <t>Augmented Analytics in BFSI Market to Witness Significant Growth with ~24.4% CAGR by 2032 | IBM Corporation</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMitgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9zYWxlcy1wZXJmb3JtYW5jZS1tYW5hZ2VtZW50LXNwbS1tYXJrZXQtYnJlYWtpbmctbmV3LWdyb3VuZHMtYW5kLXRvdWNoLW5ldy1sZXZlbC1pbi11cGNvbWluZy15ZWFyLWJ5LXNhcC1zYWxlc2ZvcmNlLWNvbS1pYm0tb3JhY2xlLzgxNjY0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMinQFodHRwczovL3d3dy53aGF0ZWNoLmNvbS9vZy9tYXJrZXRzLXJlc2VhcmNoL2l0Lzg0MjMyMy1hdWdtZW50ZWQtYW5hbHl0aWNzLWluLWJmc2ktbWFya2V0LXRvLXdpdG5lc3Mtc2lnbmlmaWNhbnQtZ3Jvd3RoLXdpdGgtMjQtNC1jYWdyLWJ5LTIwMzItaWJtLWNvcnBvcmF0aW9u0gGhAWh0dHBzOi8vd3d3LndoYXRlY2guY29tL29nL21hcmtldHMtcmVzZWFyY2gvaXQvODQyMzIzLWF1Z21lbnRlZC1hbmFseXRpY3MtaW4tYmZzaS1tYXJrZXQtdG8td2l0bmVzcy1zaWduaWZpY2FudC1ncm93dGgtd2l0aC0yNC00LWNhZ3ItYnktMjAzMi1pYm0tY29ycG9yYXRpb24vYW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>Network Diagnostic Tool NDT Market Scope and overview, To Develop with Increased Global Emphasis on ...</t>
+          <t>Lynn Conway, microchip pioneer who overcame transgender prejudice, dies aged 86</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMizwFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9uZXR3b3JrLWRpYWdub3N0aWMtdG9vbC1uZHQtbWFya2V0LXNjb3BlLWFuZC1vdmVydmlldy10by1kZXZlbG9wLXdpdGgtaW5jcmVhc2VkLWdsb2JhbC1lbXBoYXNpcy1vbi1pbmR1c3RyaWFsaXphdGlvbi0yMDMxLWlibS1taWNyb3NvZnQtZWRzLWxvY2toZWVkLW1hcnRpbi83MjI5OC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiAFodHRwczovL3d3dy5leHByZXNzYW5kc3Rhci5jb20vbmV3cy93b3JsZC1uZXdzLzIwMjQvMDYvMTQvbHlubi1jb253YXktbWljcm9jaGlwLXBpb25lZXItd2hvLW92ZXJjYW1lLXRyYW5zZ2VuZGVyLXByZWp1ZGljZS1kaWVzLWFnZWQtODYv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>Blade Server Solutions Market Growing Massively by Cisco, Dell, HP, IBM – TIMC</t>
+          <t>United Advisor Group LLC Acquires New Position in International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LnRoZWluZGlhbm1vdmllY2hhbm5lbC5jb20vbWVkaWEvYmxhZGUtc2VydmVyLXNvbHV0aW9ucy1tYXJrZXQtZ3Jvd2luZy1tYXNzaXZlbHktYnktY2lzY28tZGVsbC1ocC1pYm0vODIwNDQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiiQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTQvdW5pdGVkLWFkdmlzb3ItZ3JvdXAtbGxjLWFjcXVpcmVzLW5ldy1wb3NpdGlvbi1pbi1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvLW55c2VpYm0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>Natural Language Processing Platform Market to Make Great Impact in Near Future over 2031 Amazon, Baidu, Google ...</t>
+          <t>DC Circ. Says 'Piggybacking' Can't Save IBM Bias Claims</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMipQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9uYXR1cmFsLWxhbmd1YWdlLXByb2Nlc3NpbmctcGxhdGZvcm0tbWFya2V0LXRvLW1ha2UtZ3JlYXQtaW1wYWN0LWluLW5lYXItZnV0dXJlLW92ZXItMjAzMS1hbWF6b24tYmFpZHUtZ29vZ2xlLWlibS83Mjg5MC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigAFodHRwczovL3d3dy5sYXczNjAuY29tL2VtcGxveW1lbnQtYXV0aG9yaXR5L2Rpc2NyaW1pbmF0aW9uL2FydGljbGVzLzE4NDgzODIvZGMtY2lyYy1zYXlzLXBpZ2d5YmFja2luZy1jYW4tdC1zYXZlLWlibS1iaWFzLWNsYWltc9IBQGh0dHBzOi8vd3d3LmxhdzM2MC5jb20vZW1wbG95bWVudC1hdXRob3JpdHkvYW1wL2FydGljbGVzLzE4NDgzODI?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>Expat: Multiple vulnerabilities allow denial of service</t>
+          <t>Kerala partners with IBM to host global conclave on Gen AI | Tap to know more | Inshorts</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 14:15:06.718936</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiZGh0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9leHBhdC1tdWx0aXBsZS12dWxuZXJhYmlsaXRpZXMtYWxsb3ctZGVuaWFsLW9mLXNlcnZpY2UtMi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiZWh0dHBzOi8vaW5zaG9ydHMuY29tL2VuL25ld3Mva2VyYWxhLXBhcnRuZXJzLXdpdGgtaWJtLXRvLWhvc3QtZ2xvYmFsLWNvbmNsYXZlLW9uLWdlbi1haS0xNzE4MzM5ODcyMDU30gFpaHR0cHM6Ly9pbnNob3J0cy5jb20vZW4vYW1wX25ld3Mva2VyYWxhLXBhcnRuZXJzLXdpdGgtaWJtLXRvLWhvc3QtZ2xvYmFsLWNvbmNsYXZlLW9uLWdlbi1haS0xNzE4MzM5ODcyMDU3?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>Fan Data Analytics Market Scope and overview, To Develop with Increased Global Emphasis on Industrialization 2031 ...</t>
+          <t>McDonald's is ending its drive-thru AI test</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-14 18:13:16.593704</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMi0QFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9mYW4tZGF0YS1hbmFseXRpY3MtbWFya2V0LXNjb3BlLWFuZC1vdmVydmlldy10by1kZXZlbG9wLXdpdGgtaW5jcmVhc2VkLWdsb2JhbC1lbXBoYXNpcy1vbi1pbmR1c3RyaWFsaXphdGlvbi0yMDMxLWRlbGwtaW5jLXNhcC1zZS1pYm0tY29ycG9yYXRpb24tZGF0YW1lZXItaW5jLzc4NjcwL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiV2h0dHBzOi8vcmVzdGF1cmFudGJ1c2luZXNzb25saW5lLmNvbS90ZWNobm9sb2d5L21jZG9uYWxkcy1lbmRpbmctaXRzLWRyaXZlLXRocnUtYWktdGVzdNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>Supply Chain Digitization Technology Market Growing Massively by SAP SE, Microsoft, IBM, Veeva – TIMC</t>
+          <t>International Business Machines Co. (NYSE:IBM) Shares Bought by Bragg Financial Advisors Inc</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.707990</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL3N1cHBseS1jaGFpbi1kaWdpdGl6YXRpb24tdGVjaG5vbG9neS1tYXJrZXQtZ3Jvd2luZy1tYXNzaXZlbHktYnktc2FwLXNlLW1pY3Jvc29mdC1pYm0tdmVldmEvODE2OTIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTQvaW50ZXJuYXRpb25hbC1idXNpbmVzcy1tYWNoaW5lcy1jby1ueXNlaWJtLXNoYXJlcy1ib3VnaHQtYnktYnJhZ2ctZmluYW5jaWFsLWFkdmlzb3JzLWluYy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>Intel Ethernet Controller: Security warning about a number of IT vulnerabilities</t>
+          <t>Options Solutions LLC Increases Holdings in International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.707990</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9pbnRlbC1ldGhlcm5ldC1jb250cm9sbGVyLXNlY3VyaXR5LXdhcm5pbmctYWJvdXQtYS1udW1iZXItb2YtaXQtdnVsbmVyYWJpbGl0aWVzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTUvb3B0aW9ucy1zb2x1dGlvbnMtbGxjLWluY3JlYXNlcy1ob2xkaW5ncy1pbi1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvLW55c2VpYm0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>ICT Investment Market Size 2024: Global Share and Industry Analysis by 2031 | Microsoft, IBM, EMC, Dell – TIMC</t>
+          <t>IBM and Japan institute team up to develop next-gen quantum computer</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.707990</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMilQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9pY3QtaW52ZXN0bWVudC1tYXJrZXQtc2l6ZS0yMDI0LWdsb2JhbC1zaGFyZS1hbmQtaW5kdXN0cnktYW5hbHlzaXMtYnktMjAzMS1taWNyb3NvZnQtaWJtLWVtYy1kZWxsLzc5NzUyL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMicGh0dHBzOi8vYXNpYS5uaWtrZWkuY29tL0J1c2luZXNzL1RlY2hub2xvZ3kvSUJNLWFuZC1KYXBhbi1pbnN0aXR1dGUtdGVhbS11cC10by1kZXZlbG9wLW5leHQtZ2VuLXF1YW50dW0tY29tcHV0ZXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>Computing pioneer Lynn Conway dies aged 86</t>
+          <t>What Is the Levelized Cost of Energy (LCOE)?</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.707990</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiRmh0dHBzOi8vd3d3Lm91dGlucGVydGguY29tL2NvbXB1dGluZy1waW9uZWVyLWx5bm4tY29ud2F5LWRpZXMtYWdlZC04Ni_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiOWh0dHBzOi8vd3d3LmlibS5jb20vdGhpbmsvdG9waWNzL2xldmVsaXplZC1jb3N0LW9mLWVuZXJnedIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>Who Is The Father of India's Stock Market? Not Tata Or Ambani, But A Surprising Name Revealed By Ramesh Damani</t>
+          <t>IBM (IBM) Dips More Than Broader Markets: What You Should Know</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.707990</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiswFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL2J1c2luZXNzLWVjb25vbXkvbWFya2V0cy93aG8taXMtdGhlLWZhdGhlci1vZi1pbmRpYXMtc3RvY2stbWFya2V0LW5vdC10YXRhLW9yLWFtYmFuaS1idXQtYS1zdXJwcmlzaW5nLW5hbWUtcmV2ZWFsZWQtYnktcmFtZXNoLWRhbWFuaS1hcnRpY2xlLTExMTAxNTcxOdIBtwFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL2J1c2luZXNzLWVjb25vbXkvbWFya2V0cy93aG8taXMtdGhlLWZhdGhlci1vZi1pbmRpYXMtc3RvY2stbWFya2V0LW5vdC10YXRhLW9yLWFtYmFuaS1idXQtYS1zdXJwcmlzaW5nLW5hbWUtcmV2ZWFsZWQtYnktcmFtZXNoLWRhbWFuaS1hcnRpY2xlLTExMTAxNTcxOS9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiVGh0dHBzOi8vYXUubGlmZXN0eWxlLnlhaG9vLmNvbS9maW5hbmNlL25ld3MvaWJtLWlibS1kaXBzLW1vcmUtYnJvYWRlci0yMjQ1MTA2NjMuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>Conversational Intelligence Software Market Set for Explosive Growth | IBM, Narrativa, Retresco, Drift</t>
+          <t>Northwest Bank &amp; Trust Co Makes New Investment in International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.707990</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3Lm5ld3N0cmFpbC5jb20vY29udmVyc2F0aW9uYWwtaW50ZWxsaWdlbmNlLXNvZnR3YXJlLW1hcmtldC1zZXQtZm9yLWV4cGxvc2l2ZS1ncm93dGgtaWJtLW5hcnJhdGl2YS1yZXRyZXNjby1kcmlmdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXNlYy1maWxpbmctMjAyNC0wNi0xNS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>Semiconductor Advanced Process Technologies Market with Tremendous growth by 2031 – Apple, IBM, Intel ...</t>
+          <t>Orangetown Accedes To "Emergency" Request From Developer Who Wants To Build 342 Units At Former IBM/HNA ...</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.718936</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMingFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9zZW1pY29uZHVjdG9yLWFkdmFuY2VkLXByb2Nlc3MtdGVjaG5vbG9naWVzLW1hcmtldC13aXRoLXRyZW1lbmRvdXMtZ3Jvd3RoLWJ5LTIwMzEtYXBwbGUtaWJtLWludGVsLXF1YWxjb21tLzc1OTAwL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMipAFodHRwczovL3JjYml6am91cm5hbC5jb20vMjAyNC8wNi8xNS9vcmFuZ2V0b3duLWFjY2VkZXMtdG8tZW1lcmdlbmN5LXJlcXVlc3QtZnJvbS1kZXZlbG9wZXItd2hvLXdhbnRzLXRvLWJ1aWxkLTM0Mi11bml0cy1hdC1mb3JtZXItaWJtLWhuYS1wYWxpc2FkZXMtdHJhaW5pbmctY2VudGVyL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>Bug Tracking for Software Market Breaking New Grounds and Touch New Level in upcoming year by Atlassian, IBM ...</t>
+          <t>Able Wealth Management LLC Purchases Shares of 419 International Business Machines Co. (NYSE:IBM)</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 14:15:06.718936</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiuAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL2J1Zy10cmFja2luZy1mb3Itc29mdHdhcmUtbWFya2V0LWJyZWFraW5nLW5ldy1ncm91bmRzLWFuZC10b3VjaC1uZXctbGV2ZWwtaW4tdXBjb21pbmcteWVhci1ieS1hdGxhc3NpYW4taWJtLWpldGJyYWlucy16b2hvY29ycG9yYXRpb24vNzg1NjIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiigFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTUvYWJsZS13ZWFsdGgtbWFuYWdlbWVudC1sbGMtcHVyY2hhc2VzLXNoYXJlcy1vZi00MTktaW50ZXJuYXRpb25hbC1idXNpbmVzcy1tYWNoaW5lcy1jby1ueXNlaWJtLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>Building strategic partnerships in e-commerce: Collaboration for growth</t>
+          <t>Abandoned History: Oldsmobile's Guidestar Navigation System and Other Cartography (Part V)</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiW2h0dHBzOi8vZ3VhcmRpYW4ubmcvYnVpbGRpbmctc3RyYXRlZ2ljLXBhcnRuZXJzaGlwcy1pbi1lLWNvbW1lcmNlLWNvbGxhYm9yYXRpb24tZm9yLWdyb3d0aC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMitwFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL21vbmV5L2NvbXBhbmllcy9hYmFuZG9uZWQtaGlzdG9yeS1vbGRzbW9iaWxlLXMtZ3VpZGVzdGFyLW5hdmlnYXRpb24tc3lzdGVtLWFuZC1vdGhlci1jYXJ0b2dyYXBoeS1wYXJ0LXYvYXItQUExbHpKSmM_aXRlbT1mbGlnaHRzcHJnLXRpcHN1YnNjLXYxYT9zZWFzb249MjAyNC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>Business Analysis Tools Market Set for Rapid Growth by 2031 – Alteryx, Inc., IBM, InCorta – TIMC</t>
+          <t>The Dividend Dukes: 3 Stocks That Will Elevate Your Portfolio's Nobility</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:08.898364</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL2J1c2luZXNzLWFuYWx5c2lzLXRvb2xzLW1hcmtldC1zZXQtZm9yLXJhcGlkLWdyb3d0aC1ieS0yMDMxLWFsdGVyeXgtaW5jLWlibS1pbmNvcnRhLzgyMDE1L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMifWh0dHBzOi8vd3d3Lm1zbi5jb20vZW4tdXMvbW9uZXkvdG9wc3RvY2tzL3RoZS1kaXZpZGVuZC1kdWtlcy0zLXN0b2Nrcy10aGF0LXdpbGwtZWxldmF0ZS15b3VyLXBvcnRmb2xpby1zLW5vYmlsaXR5L2FyLUJCMW9hQWVi0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>Options Solutions LLC Increases Holdings in International Business Machines Co. (NYSE:IBM)</t>
+          <t>Raymond G. Guillet</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:16.600323</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMigwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTUvb3B0aW9ucy1zb2x1dGlvbnMtbGxjLWluY3JlYXNlcy1ob2xkaW5ncy1pbi1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvLW55c2VpYm0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiP2h0dHBzOi8vd3d3LnJlcC1hbS5jb20vb2JpdHVhcmllcy8yMDI0LzA2LzE1L3JheW1vbmQtZy1ndWlsbGV0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>International Business Machines Co. (NYSE:IBM) Shares Bought by Bragg Financial Advisors Inc</t>
+          <t>Lynn Conway, Microchip Pioneer who Overcame Transgender Discrimination, Dies at 86 | EDGE United States</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:16.600323</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMihQFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTQvaW50ZXJuYXRpb25hbC1idXNpbmVzcy1tYWNoaW5lcy1jby1ueXNlaWJtLXNoYXJlcy1ib3VnaHQtYnktYnJhZ2ctZmluYW5jaWFsLWFkdmlzb3JzLWluYy5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiLWh0dHBzOi8vd3d3LmVkZ2VtZWRpYW5ldHdvcmsuY29tL3N0b3J5LzMzMzgyOdIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>IBM and Japan institute team up to develop next-gen quantum computer</t>
+          <t>Thomas Stone Obituary (2024) - Savannah, GA - Fox &amp; Weeks Funeral Directors - Hodgson Chapel</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>2024-06-15 18:13:16.600323</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMicGh0dHBzOi8vYXNpYS5uaWtrZWkuY29tL0J1c2luZXNzL1RlY2hub2xvZ3kvSUJNLWFuZC1KYXBhbi1pbnN0aXR1dGUtdGVhbS11cC10by1kZXZlbG9wLW5leHQtZ2VuLXF1YW50dW0tY29tcHV0ZXLSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiS2h0dHBzOi8vd3d3LmxlZ2FjeS5jb20vdXMvb2JpdHVhcmllcy9uYW1lL3Rob21hcy1zdG9uZS1vYml0dWFyeT9pZD01NTM1MzAzNNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>McDonalds is removing its AI drive-thru voice ordering system from over 100 restaurants after its mishaps went</t>
+          <t>3 Tech Stocks With A History Of Reliable Dividends</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>2024-06-15 19:13:08.889417</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiuQFodHRwczovL3d3dy5idXNpbmVzc2luc2lkZXIuaW4vcmV0YWlsL25ld3MvbWNkb25hbGRzLWlzLXJlbW92aW5nLWl0cy1haS1kcml2ZS10aHJ1LXZvaWNlLW9yZGVyaW5nLXN5c3RlbS1mcm9tLW92ZXItMTAwLXJlc3RhdXJhbnRzLWFmdGVyLWl0cy1taXNoYXBzLXdlbnQtdmlyYWwvYXJ0aWNsZXNob3cvMTExMDQyODgxLmNtc9IBvQFodHRwczovL3d3dy5idXNpbmVzc2luc2lkZXIuaW4vcmV0YWlsL25ld3MvbWNkb25hbGRzLWlzLXJlbW92aW5nLWl0cy1haS1kcml2ZS10aHJ1LXZvaWNlLW9yZGVyaW5nLXN5c3RlbS1mcm9tLW92ZXItMTAwLXJlc3RhdXJhbnRzLWFmdGVyLWl0cy1taXNoYXBzLXdlbnQtdmlyYWwvYW1wX2FydGljbGVzaG93LzExMTA0Mjg4MS5jbXM?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiT2h0dHBzOi8vdWsuZmluYW5jZS55YWhvby5jb20vbmV3cy8zLXRlY2gtc3RvY2tzLWhpc3RvcnktcmVsaWFibGUtMTcxMjM0NzM0Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>Fans Were Furious With Fox's Broadcast Decision During Euros Today</t>
+          <t>How to make boot media for PowerPC Macs on modern hardware - Mac Software Discussions on AppleInsider Forums</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>2024-06-15 19:13:08.889417</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiYWh0dHBzOi8vdGhlc3B1bi5jb20vdG9wLXN0b3JpZXMvZmFucy13ZXJlLWZ1cmlvdXMtd2l0aC1mb3hzLWJyb2FkY2FzdC1kZWNpc2lvbi1kdXJpbmctZXVyb3MtdG9kYXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiMWh0dHBzOi8vZm9ydW1zLmFwcGxlaW5zaWRlci5jb20vZGlzY3Vzc2lvbi8yMzY3NjPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>Northwest Bank &amp; Trust Co Makes New Investment in International Business Machines Co. (NYSE:IBM)</t>
+          <t>Red Hat Launches RHEL AI and InstructLab to Bring Generative AI to the Enterprise</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>2024-06-15 20:13:08.889417</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXNlYy1maWxpbmctMjAyNC0wNi0xNS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMiemh0dHBzOi8vd3d3Lmdsb2JhbHZpbGxhZ2VzcGFjZS5jb20vdGVjaC9yZWQtaGF0LWxhdW5jaGVzLXJoZWwtYWktYW5kLWluc3RydWN0bGFiLXRvLWJyaW5nLWdlbmVyYXRpdmUtYWktdG8tdGhlLWVudGVycHJpc2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>Lynn Conway: Remembering the Legacy of a Computing Pioneer and Transgender Advocate</t>
+          <t>Top multinational companies bet big on Hyderabad's commercial real estate market, lease 8.7 lakh sq ft of office space</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>2024-06-15 22:13:08.898364</t>
+          <t>2024-06-15 18:13:08.889417</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>news.google.com/articles/CBMibmh0dHBzOi8vd3d3LndpcmVuZXdzZmF4LmNvbS9seW5uLWNvbndheS1yZW1lbWJlcmluZy10aGUtbGVnYWN5LW9mLWEtY29tcHV0aW5nLXBpb25lZXItYW5kLXRyYW5zZ2VuZGVyLWFkdm9jYXRl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+          <t>news.google.com/articles/CBMisgFodHRwczovL3d3dy5tc24uY29tL2VuLWluL25ld3MvSW5kaWEvdG9wLW11bHRpbmF0aW9uYWwtY29tcGFuaWVzLWJldC1iaWctb24taHlkZXJhYmFkLXMtY29tbWVyY2lhbC1yZWFsLWVzdGF0ZS1tYXJrZXQtbGVhc2UtOC03LWxha2gtc3EtZnQtb2Ytb2ZmaWNlLXNwYWNlL2FyLUJCMW8xYjhnP29jaWQ9TEVOREhQ0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
+          <t>Lynn Conway has passed.</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.889417</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiSmh0dHBzOi8vd3d3LmRhaWx5a29zLmNvbS9zdG9yaWVzLzIwMjQvNi8xNS8yMjQ2ODQxLy1MeW5uLUNvbndheS1oYXMtcGFzc2Vk0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Taylor Financial Group Inc. Takes $209000 Position in International Business Machines Co. (NYSE:IBM)</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.889417</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTUvdGF5bG9yLWZpbmFuY2lhbC1ncm91cC1pbmMtdGFrZXMtMjA5MDAwLXBvc2l0aW9uLWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Lynn Conway, Computing Pioneer and Transgender Advocate, Dies at 86</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.889417</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiQ2h0dHBzOi8vd3d3Lm55dGltZXMuY29tLzIwMjQvMDYvMTUvdGVjaG5vbG9neS9seW5uLWNvbndheS1kZWFkLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Stock market today: Dow sidesteps tech wreck to keep winning streak alive</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.889417</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vY2Euc3R5bGUueWFob28uY29tL3N0eWxlL3N0b2NrLW1hcmtldC10b2RheS1kb3ctc2lkZXN0ZXBzLTE2MTcwMzI5Ni5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Natural Language Processing Platform Market to Make Great Impact in Near Future over 2031 Amazon, Baidu, Google ...</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMipQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9uYXR1cmFsLWxhbmd1YWdlLXByb2Nlc3NpbmctcGxhdGZvcm0tbWFya2V0LXRvLW1ha2UtZ3JlYXQtaW1wYWN0LWluLW5lYXItZnV0dXJlLW92ZXItMjAzMS1hbWF6b24tYmFpZHUtZ29vZ2xlLWlibS83Mjg5MC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Expat: Multiple vulnerabilities allow denial of service</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9leHBhdC1tdWx0aXBsZS12dWxuZXJhYmlsaXRpZXMtYWxsb3ctZGVuaWFsLW9mLXNlcnZpY2UtMi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>GDPR Services Market Booming Worldwide with Latest Trend and Future scope with Top Key Players- IBM, Veritas ...</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMirAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9nZHByLXNlcnZpY2VzLW1hcmtldC1ib29taW5nLXdvcmxkd2lkZS13aXRoLWxhdGVzdC10cmVuZC1hbmQtZnV0dXJlLXNjb3BlLXdpdGgtdG9wLWtleS1wbGF5ZXJzLWlibS12ZXJpdGFzLWF3cy1taWNyb3NvZnQvNzExNDUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>IT safety: Linux is weak - expat IT safety alert replace (vulnerability: medium)</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidmh0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9pdC1zYWZldHktbGludXgtaXMtd2Vhay1leHBhdC1pdC1zYWZldHktYWxlcnQtcmVwbGFjZS12dWxuZXJhYmlsaXR5LW1lZGl1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Anything-as-a-Service Market will touch a new level in upcoming year with Top Key Players like Cisco, Google, IBM ...</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMirQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9hbnl0aGluZy1hcy1hLXNlcnZpY2UtbWFya2V0LXdpbGwtdG91Y2gtYS1uZXctbGV2ZWwtaW4tdXBjb21pbmcteWVhci13aXRoLXRvcC1rZXktcGxheWVycy1saWtlLWNpc2NvLWdvb2dsZS1pYm0tbWljcm9zb2Z0LzcxMTQ3L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Sales Performance Management (SPM) Market Breaking New Grounds and Touch New Level in upcoming year by ...</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMitgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9zYWxlcy1wZXJmb3JtYW5jZS1tYW5hZ2VtZW50LXNwbS1tYXJrZXQtYnJlYWtpbmctbmV3LWdyb3VuZHMtYW5kLXRvdWNoLW5ldy1sZXZlbC1pbi11cGNvbWluZy15ZWFyLWJ5LXNhcC1zYWxlc2ZvcmNlLWNvbS1pYm0tb3JhY2xlLzgxNjY0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>Network Diagnostic Tool NDT Market Scope and overview, To Develop with Increased Global Emphasis on ...</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMizwFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9uZXR3b3JrLWRpYWdub3N0aWMtdG9vbC1uZHQtbWFya2V0LXNjb3BlLWFuZC1vdmVydmlldy10by1kZXZlbG9wLXdpdGgtaW5jcmVhc2VkLWdsb2JhbC1lbXBoYXNpcy1vbi1pbmR1c3RyaWFsaXphdGlvbi0yMDMxLWlibS1taWNyb3NvZnQtZWRzLWxvY2toZWVkLW1hcnRpbi83MjI5OC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Semiconductor Advanced Process Technologies Market with Tremendous growth by 2031 – Apple, IBM, Intel ...</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMingFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9zZW1pY29uZHVjdG9yLWFkdmFuY2VkLXByb2Nlc3MtdGVjaG5vbG9naWVzLW1hcmtldC13aXRoLXRyZW1lbmRvdXMtZ3Jvd3RoLWJ5LTIwMzEtYXBwbGUtaWJtLWludGVsLXF1YWxjb21tLzc1OTAwL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Intel Ethernet Controller: Security warning about a number of IT vulnerabilities</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMie2h0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9pbnRlbC1ldGhlcm5ldC1jb250cm9sbGVyLXNlY3VyaXR5LXdhcm5pbmctYWJvdXQtYS1udW1iZXItb2YtaXQtdnVsbmVyYWJpbGl0aWVzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Blade Server Solutions Market Growing Massively by Cisco, Dell, HP, IBM – TIMC</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LnRoZWluZGlhbm1vdmllY2hhbm5lbC5jb20vbWVkaWEvYmxhZGUtc2VydmVyLXNvbHV0aW9ucy1tYXJrZXQtZ3Jvd2luZy1tYXNzaXZlbHktYnktY2lzY28tZGVsbC1ocC1pYm0vODIwNDQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Supply Chain Digitization Technology Market Growing Massively by SAP SE, Microsoft, IBM, Veeva – TIMC</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMijgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL3N1cHBseS1jaGFpbi1kaWdpdGl6YXRpb24tdGVjaG5vbG9neS1tYXJrZXQtZ3Jvd2luZy1tYXNzaXZlbHktYnktc2FwLXNlLW1pY3Jvc29mdC1pYm0tdmVldmEvODE2OTIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Bug Tracking for Software Market Breaking New Grounds and Touch New Level in upcoming year by Atlassian, IBM ...</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiuAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL2J1Zy10cmFja2luZy1mb3Itc29mdHdhcmUtbWFya2V0LWJyZWFraW5nLW5ldy1ncm91bmRzLWFuZC10b3VjaC1uZXctbGV2ZWwtaW4tdXBjb21pbmcteWVhci1ieS1hdGxhc3NpYW4taWJtLWpldGJyYWlucy16b2hvY29ycG9yYXRpb24vNzg1NjIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Computing pioneer Lynn Conway dies aged 86</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiRmh0dHBzOi8vd3d3Lm91dGlucGVydGguY29tL2NvbXB1dGluZy1waW9uZWVyLWx5bm4tY29ud2F5LWRpZXMtYWdlZC04Ni_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Who Is The Father of India's Stock Market? Not Tata Or Ambani, But A Surprising Name Revealed By Ramesh Damani</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiswFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL2J1c2luZXNzLWVjb25vbXkvbWFya2V0cy93aG8taXMtdGhlLWZhdGhlci1vZi1pbmRpYXMtc3RvY2stbWFya2V0LW5vdC10YXRhLW9yLWFtYmFuaS1idXQtYS1zdXJwcmlzaW5nLW5hbWUtcmV2ZWFsZWQtYnktcmFtZXNoLWRhbWFuaS1hcnRpY2xlLTExMTAxNTcxOdIBtwFodHRwczovL3d3dy50aW1lc25vd25ld3MuY29tL2J1c2luZXNzLWVjb25vbXkvbWFya2V0cy93aG8taXMtdGhlLWZhdGhlci1vZi1pbmRpYXMtc3RvY2stbWFya2V0LW5vdC10YXRhLW9yLWFtYmFuaS1idXQtYS1zdXJwcmlzaW5nLW5hbWUtcmV2ZWFsZWQtYnktcmFtZXNoLWRhbWFuaS1hcnRpY2xlLTExMTAxNTcxOS9hbXA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Conversational Intelligence Software Market Set for Explosive Growth | IBM, Narrativa, Retresco, Drift</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifGh0dHBzOi8vd3d3Lm5ld3N0cmFpbC5jb20vY29udmVyc2F0aW9uYWwtaW50ZWxsaWdlbmNlLXNvZnR3YXJlLW1hcmtldC1zZXQtZm9yLWV4cGxvc2l2ZS1ncm93dGgtaWJtLW5hcnJhdGl2YS1yZXRyZXNjby1kcmlmdC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>Business Analysis Tools Market Set for Rapid Growth by 2031 – Alteryx, Inc., IBM, InCorta – TIMC</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL2J1c2luZXNzLWFuYWx5c2lzLXRvb2xzLW1hcmtldC1zZXQtZm9yLXJhcGlkLWdyb3d0aC1ieS0yMDMxLWFsdGVyeXgtaW5jLWlibS1pbmNvcnRhLzgyMDE1L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Building strategic partnerships in e-commerce: Collaboration for growth</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiW2h0dHBzOi8vZ3VhcmRpYW4ubmcvYnVpbGRpbmctc3RyYXRlZ2ljLXBhcnRuZXJzaGlwcy1pbi1lLWNvbW1lcmNlLWNvbGxhYm9yYXRpb24tZm9yLWdyb3d0aC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>ICT Investment Market Size 2024: Global Share and Industry Analysis by 2031 | Microsoft, IBM, EMC, Dell – TIMC</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMilQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9pY3QtaW52ZXN0bWVudC1tYXJrZXQtc2l6ZS0yMDI0LWdsb2JhbC1zaGFyZS1hbmQtaW5kdXN0cnktYW5hbHlzaXMtYnktMjAzMS1taWNyb3NvZnQtaWJtLWVtYy1kZWxsLzc5NzUyL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>IT safety: Linux, macOS X and UNIX are threatened - IT safety alert replace for Node.js (danger: medium)</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy5icmVha2luZ2xhdGVzdC5uZXdzL3RlY2hub2xvZ3kvaXQtc2FmZXR5LWxpbnV4LW1hY29zLXgtYW5kLXVuaXgtYXJlLXRocmVhdGVuZWQtaXQtc2FmZXR5LWFsZXJ0LXJlcGxhY2UtZm9yLW5vZGUtanMtZGFuZ2VyLW1lZGl1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Fan Data Analytics Market Scope and overview, To Develop with Increased Global Emphasis on Industrialization 2031 ...</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>2024-06-15 18:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMi0QFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9mYW4tZGF0YS1hbmFseXRpY3MtbWFya2V0LXNjb3BlLWFuZC1vdmVydmlldy10by1kZXZlbG9wLXdpdGgtaW5jcmVhc2VkLWdsb2JhbC1lbXBoYXNpcy1vbi1pbmR1c3RyaWFsaXphdGlvbi0yMDMxLWRlbGwtaW5jLXNhcC1zZS1pYm0tY29ycG9yYXRpb24tZGF0YW1lZXItaW5jLzc4NjcwL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>McDonalds is removing its AI drive-thru voice ordering system from over 100 restaurants after its mishaps went</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>2024-06-15 19:13:08.889417</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiuQFodHRwczovL3d3dy5idXNpbmVzc2luc2lkZXIuaW4vcmV0YWlsL25ld3MvbWNkb25hbGRzLWlzLXJlbW92aW5nLWl0cy1haS1kcml2ZS10aHJ1LXZvaWNlLW9yZGVyaW5nLXN5c3RlbS1mcm9tLW92ZXItMTAwLXJlc3RhdXJhbnRzLWFmdGVyLWl0cy1taXNoYXBzLXdlbnQtdmlyYWwvYXJ0aWNsZXNob3cvMTExMDQyODgxLmNtc9IBvQFodHRwczovL3d3dy5idXNpbmVzc2luc2lkZXIuaW4vcmV0YWlsL25ld3MvbWNkb25hbGRzLWlzLXJlbW92aW5nLWl0cy1haS1kcml2ZS10aHJ1LXZvaWNlLW9yZGVyaW5nLXN5c3RlbS1mcm9tLW92ZXItMTAwLXJlc3RhdXJhbnRzLWFmdGVyLWl0cy1taXNoYXBzLXdlbnQtdmlyYWwvYW1wX2FydGljbGVzaG93LzExMTA0Mjg4MS5jbXM?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>Fans Were Furious With Fox's Broadcast Decision During Euros Today</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>2024-06-15 19:13:08.889417</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiYWh0dHBzOi8vdGhlc3B1bi5jb20vdG9wLXN0b3JpZXMvZmFucy13ZXJlLWZ1cmlvdXMtd2l0aC1mb3hzLWJyb2FkY2FzdC1kZWNpc2lvbi1kdXJpbmctZXVyb3MtdG9kYXnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Lynn Conway: Remembering the Legacy of a Computing Pioneer and Transgender Advocate</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>2024-06-15 22:13:08.898364</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMibmh0dHBzOi8vd3d3LndpcmVuZXdzZmF4LmNvbS9seW5uLWNvbndheS1yZW1lbWJlcmluZy10aGUtbGVnYWN5LW9mLWEtY29tcHV0aW5nLXBpb25lZXItYW5kLXRyYW5zZ2VuZGVyLWFkdm9jYXRl0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
           <t>FM Software Market Growing Massively by IBM, Oracle, SAP, Archibus – TIMC</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
+      <c r="B194" t="inlineStr">
         <is>
           <t>2024-06-15 23:13:08.898364</t>
         </is>
       </c>
-      <c r="C167" t="inlineStr">
+      <c r="C194" t="inlineStr">
         <is>
           <t>news.google.com/articles/CBMicmh0dHBzOi8vd3d3LnRoZWluZGlhbm1vdmllY2hhbm5lbC5jb20vbWVkaWEvZm0tc29mdHdhcmUtbWFya2V0LWdyb3dpbmctbWFzc2l2ZWx5LWJ5LWlibS1vcmFjbGUtc2FwLWFyY2hpYnVzLzgyMzYwL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Smart Contracts Market Analysis, Research Study With IBM, Oracle, Chainlink, Microsoft – TIMC</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>2024-06-16 14:15:06.718936</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9zbWFydC1jb250cmFjdHMtbWFya2V0LWFuYWx5c2lzLXJlc2VhcmNoLXN0dWR5LXdpdGgtaWJtLW9yYWNsZS1jaGFpbmxpbmstbWljcm9zb2Z0Lzg3NjA5L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>What is an AI accelerator?</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiL2h0dHBzOi8vd3d3LmlibS5jb20vdGhpbmsvdG9waWNzL2FpLWFjY2VsZXJhdG9y0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Tech Tuesdays: StockX Battles Counterfeits + IBM on Gen AI Use</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUmh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vdGVjaC10dWVzZGF5cy1zdG9ja3gtYmF0dGxlcy1jb3VudGVyZmVpdHMtMTQwMDIxNzEzLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>AMD CEO Lisa Su reminisces about designing the PS3's infamous Cell processor during her time at IBM</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMimQFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL25ld3MvdGVjaG5vbG9neS9hbWQtY2VvLWxpc2Etc3UtcmVtaW5pc2Nlcy1hYm91dC1kZXNpZ25pbmctdGhlLXBzMy1zLWluZmFtb3VzLWNlbGwtcHJvY2Vzc29yLWR1cmluZy1oZXItdGltZS1hdC1pYm0vYXItQkIxb2FiN2TSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>McDonald's removing AI-powered voice-order technology from drive-thrus</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiVmh0dHBzOi8vd3d3LmJ1c2luZXNzaW5zaWRlci5jb20vbWNkb25hbGRzLWFpLXZvaWNlLW9yZGVyLXRlY2hub2xvZ3ktZHJpdmUtdGhydXMtMjAyNC020gFaaHR0cHM6Ly93d3cuYnVzaW5lc3NpbnNpZGVyLmNvbS9tY2RvbmFsZHMtYWktdm9pY2Utb3JkZXItdGVjaG5vbG9neS1kcml2ZS10aHJ1cy0yMDI0LTY_YW1w?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>8,018 Shares in International Business Machines Co. (NYSE:IBM) Bought by Sierra Summit Advisors LLC</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vd3d3Lm1hcmtldGJlYXQuY29tL2luc3RhbnQtYWxlcnRzL255c2UtaWJtLXNlYy1maWxpbmctMjAyNC0wNi0xNi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>International Business Machines (NYSE:IBM) Shares Down 0.7%</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZmh0dHBzOi8vd3d3LmRlZmVuc2V3b3JsZC5uZXQvMjAyNC8wNi8xNi9pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLW55c2VpYm0tc2hhcmVzLWRvd24tMC03LTIuaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Napa Wealth Management Invests $2.79 Million in International Business Machines Co. (NYSE:IBM)</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihgFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTYvbmFwYS13ZWFsdGgtbWFuYWdlbWVudC1pbnZlc3RzLTItNzktbWlsbGlvbi1pbi1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvLW55c2VpYm0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>McDonald's will stop testing AI to take drive-thru orders, for now</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZGh0dHBzOi8vd3d3LnRoZXZlcmdlLmNvbS8yMDI0LzYvMTYvMjQxNzk2NzkvbWNkb25hbGRzLWVuZGluZy1haS1jaGF0Ym90LWRyaXZlLXRocnUtb3JkZXJpbmctdGVzdC1pYm3SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Dodge &amp; Cox Sells 215 Shares of International Business Machines Co. (NYSE:IBM)</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMidWh0dHBzOi8vd3d3LmRlZmVuc2V3b3JsZC5uZXQvMjAyNC8wNi8xNi9kb2RnZS1jb3gtc2VsbHMtMjE1LXNoYXJlcy1vZi1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWNvLW55c2VpYm0uaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>IBM layoffs hit some Triangle workers, but it's unclear how many jobs will be lost</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiSWh0dHBzOi8vY2EubmV3cy55YWhvby5jb20vaWJtLWxheW9mZnMtaGl0LXRyaWFuZ2xlLXdvcmtlcnMtMTYxNTE4NzIwLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Cannes Lions 2024</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiIWh0dHBzOi8vd3d3LmlibS5jb20vZXZlbnRzL2Nhbm5lc9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Proathlete Wealth Management LLC Makes New $760000 Investment in International Business Machines Co. (NYSE ...</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.376111</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMilwFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTYvcHJvYXRobGV0ZS13ZWFsdGgtbWFuYWdlbWVudC1sbGMtbWFrZXMtbmV3LTc2MDAwMC1pbnZlc3RtZW50LWluLWludGVybmF0aW9uYWwtYnVzaW5lc3MtbWFjaGluZXMtY28tbnlzZWlibS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>Sierra Summit Advisors LLC Makes New Investment in International Business Machines Co. (NYSE:IBM)</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiigFodHRwczovL3d3dy5kZWZlbnNld29ybGQubmV0LzIwMjQvMDYvMTYvc2llcnJhLXN1bW1pdC1hZHZpc29ycy1sbGMtbWFrZXMtbmV3LWludmVzdG1lbnQtaW4taW50ZXJuYXRpb25hbC1idXNpbmVzcy1tYWNoaW5lcy1jby1ueXNlaWJtLmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Content Analytics Market Is Booming Worldwide – International Business Machines (IBM) Corporation, SAP SE, SAS ...</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMirAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL2NvbnRlbnQtYW5hbHl0aWNzLW1hcmtldC1pcy1ib29taW5nLXdvcmxkd2lkZS1pbnRlcm5hdGlvbmFsLWJ1c2luZXNzLW1hY2hpbmVzLWlibS1jb3Jwb3JhdGlvbi1zYXAtc2Utc2FzLWluc3RpdHV0ZS1vcmFjbGUvODk3NTUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Enterprise Information Archiving Market to Witness Revolutionary Growth by 2030 | Microsoft (US), HPE (US), IBM (US ...</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMipgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL2VudGVycHJpc2UtaW5mb3JtYXRpb24tYXJjaGl2aW5nLW1hcmtldC10by13aXRuZXNzLXJldm9sdXRpb25hcnktZ3Jvd3RoLWJ5LTIwMzAtbWljcm9zb2Z0LXVzLWhwZS11cy1pYm0tdXNnb29nbGUtdXMvODk2NTIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Services Oriented Architecture (SOA) Middleware Market to Witness Massive Growth by 2030 | Fujitsu Interstage ...</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMivAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL3NlcnZpY2VzLW9yaWVudGVkLWFyY2hpdGVjdHVyZS1zb2EtbWlkZGxld2FyZS1tYXJrZXQtdG8td2l0bmVzcy1tYXNzaXZlLWdyb3d0aC1ieS0yMDMwLWZ1aml0c3UtaW50ZXJzdGFnZS1oZXdsZXR0LXBhY2thcmQtaWJtLWluZm9ybWF0aWNhLzg4NTE5L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>Smart Oilfield IT Services Market to Witness Significant Incremental Opportunity Through 2024-2030 | IBM, Accenture ...</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiwwFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL3NtYXJ0LW9pbGZpZWxkLWl0LXNlcnZpY2VzLW1hcmtldC10by13aXRuZXNzLXNpZ25pZmljYW50LWluY3JlbWVudGFsLW9wcG9ydHVuaXR5LXRocm91Z2gtMjAyNC0yMDMwLWlibS1hY2NlbnR1cmUtdGF0YS1jb25zdWx0YW5jeS1zZXJ2aWNlcy13aXByby84OTg2NC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>IBM Java vulnerability: Vulnerability permits safety measures to be bypassed</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMid2h0dHBzOi8vd3d3LmJyZWFraW5nbGF0ZXN0Lm5ld3MvdGVjaG5vbG9neS9pYm0tamF2YS12dWxuZXJhYmlsaXR5LXZ1bG5lcmFiaWxpdHktcGVybWl0cy1zYWZldHktbWVhc3VyZXMtdG8tYmUtYnlwYXNzZWQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>Smart Waste Management System Market to Make Great Impact in Near Future over 2030 IBM Corporation, SAP SE ...</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMitgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL21lZGlhL3NtYXJ0LXdhc3RlLW1hbmFnZW1lbnQtc3lzdGVtLW1hcmtldC10by1tYWtlLWdyZWF0LWltcGFjdC1pbi1uZWFyLWZ1dHVyZS1vdmVyLTIwMzAtaWJtLWNvcnBvcmF0aW9uLXNhcC1zZS13YXN0ZS1tYW5hZ2VtZW50LWVuZXZvLW95Lzg5ODM0L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>McDonald's removes AI-powered voice ordering technology from drive thru</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiX2h0dHBzOi8vZmlvcnJlcG9ydHMuY29tL21jZG9uYWxkcy1yZW1vdmVzLWFpLXBvd2VyZWQtdm9pY2Utb3JkZXJpbmctdGVjaG5vbG9neS1mcm9tLWRyaXZlLXRocnUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>IT Security: Linux, MacOS X and UNIX are beneath menace - IT safety warning replace on Apache Commons (Risk ...</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>2024-06-16 19:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMimQFodHRwczovL3d3dy5icmVha2luZ2xhdGVzdC5uZXdzL3RlY2hub2xvZ3kvaXQtc2VjdXJpdHktbGludXgtbWFjb3MteC1hbmQtdW5peC1hcmUtYmVuZWF0aC1tZW5hY2UtaXQtc2FmZXR5LXdhcm5pbmctcmVwbGFjZS1vbi1hcGFjaGUtY29tbW9ucy1yaXNrLW1lZGl1bS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>McDonald's to stop testing AI to take drive-thru orders, after huge IBM partnership</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>2024-06-16 20:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifmh0dHBzOi8vd3d3LnR3ZWFrdG93bi5jb20vbmV3cy85ODg0Mi9tY2RvbmFsZHMtdG8tc3RvcC10ZXN0aW5nLWFpLXRha2UtZHJpdmUtdGhydS1vcmRlcnMtYWZ0ZXItaHVnZS1pYm0tcGFydG5lcnNoaXAvaW5kZXguaHRtbNIBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>McDonald's Is Removing Its Current AI Technology From More Than 100 Drive-Thrus</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>2024-06-16 22:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMinwFodHRwczovL3d3dy5tc24uY29tL2VuLXVzL21vbmV5L2NvbXBhbmllcy9tY2RvbmFsZC1zLWlzLXJlbW92aW5nLWl0cy1jdXJyZW50LWFpLXRlY2hub2xvZ3ktZnJvbS1tb3JlLXRoYW4tMTAwLWRyaXZlLXRocnVzL2FyLUJCMW9reUtmP29jaWQ9ZmluYW5jZS12ZXJ0aHAtZmVlZHPSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>McDonald's removes AI chatbot it partnered with IBM to use for drive-thru orders</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>2024-06-16 22:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiRWh0dHBzOi8vZ2lnYXppbmUubmV0L2dzY19uZXdzL2VuLzIwMjQwNjE3LW1jZG9uYWxkLWVuZC1kcml2ZS10aHJ1LWFpL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>McDonalds is removing its AI drive-thru voice ordering system from over 100 restaurants after its mishaps went viral</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>2024-06-16 22:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMipQFodHRwczovL3d3dy5tc24uY29tL2VuLWluL21vbmV5L25ld3MvbWNkb25hbGRzLWlzLXJlbW92aW5nLWl0cy1haS1kcml2ZS10aHJ1LXZvaWNlLW9yZGVyaW5nLXN5c3RlbS1mcm9tLW92ZXItMTAwLXJlc3RhdXJhbnRzLWFmdGVyLWl0cy1taXNoYXBzLXdlbnQtdmlyYWwvYXItQkIxb2t2ZHnSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>ITACM and ITOM Market Size 2024: Global Share and Industry Analysis by 2031 | Splunk, SolarWinds, IBM, Cicso – TIMC</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:15:06.718936</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMimgFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9pdGFjbS1hbmQtaXRvbS1tYXJrZXQtc2l6ZS0yMDI0LWdsb2JhbC1zaGFyZS1hbmQtaW5kdXN0cnktYW5hbHlzaXMtYnktMjAzMS1zcGx1bmstc29sYXJ3aW5kcy1pYm0tY2ljc28vOTA0MDAv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Smart City ICT Infrastructure Market Analysis, Research Study With Cisco, IBM, Oracle, Huawei – TIMC</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:15:06.718936</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMijQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9zbWFydC1jaXR5LWljdC1pbmZyYXN0cnVjdHVyZS1tYXJrZXQtYW5hbHlzaXMtcmVzZWFyY2gtc3R1ZHktd2l0aC1jaXNjby1pYm0tb3JhY2xlLWh1YXdlaS85MDE2Mi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>Procurement Outsourcing Market See Huge Growth for New Normal | IBM, Accenture, GEP, Infosys – TIMC</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:15:06.718936</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiiwFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9wcm9jdXJlbWVudC1vdXRzb3VyY2luZy1tYXJrZXQtc2VlLWh1Z2UtZ3Jvd3RoLWZvci1uZXctbm9ybWFsLWlibS1hY2NlbnR1cmUtZ2VwLWluZm9zeXMvOTAxNjQv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>IBM and The All England Lawn Tennis Club Launch New Generative AI Feature for Personalised Player Stories at ...</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMirgFodHRwczovL3d3dy5wcm5ld3N3aXJlLmNvbS9uZXdzLXJlbGVhc2VzL2libS1hbmQtdGhlLWFsbC1lbmdsYW5kLWxhd24tdGVubmlzLWNsdWItbGF1bmNoLW5ldy1nZW5lcmF0aXZlLWFpLWZlYXR1cmUtZm9yLXBlcnNvbmFsaXNlZC1wbGF5ZXItc3Rvcmllcy1hdC13aW1ibGVkb24tMzAyMTczNjU1Lmh0bWzSAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>General Data Protection Regulation (GDPR) Service Market Is Expected to Boom- IBM, Veritas, Amazon Web Services ...</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiqAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9nZW5lcmFsLWRhdGEtcHJvdGVjdGlvbi1yZWd1bGF0aW9uLWdkcHItc2VydmljZS1tYXJrZXQtaXMtZXhwZWN0ZWQtdG8tYm9vbS1pYm0tdmVyaXRhcy1hbWF6b24td2ViLXNlcnZpY2VzLW1pY3Jvc29mdC85MDcyOC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>IT Operation and Maintenance Software Market Recovery and Impact Analysis Report – Splunk, SolarWinds, IBM ...</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMioAFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9pdC1vcGVyYXRpb24tYW5kLW1haW50ZW5hbmNlLXNvZnR3YXJlLW1hcmtldC1yZWNvdmVyeS1hbmQtaW1wYWN0LWFuYWx5c2lzLXJlcG9ydC1zcGx1bmstc29sYXJ3aW5kcy1pYm0tY2ljc28vOTA5MzEv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence (AI) Infrastructure Market to Witness Growth Acceleration | Cisco, IBM, Intel Corporation ...</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMipwFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9hcnRpZmljaWFsLWludGVsbGlnZW5jZS1haS1pbmZyYXN0cnVjdHVyZS1tYXJrZXQtdG8td2l0bmVzcy1ncm93dGgtYWNjZWxlcmF0aW9uLWNpc2NvLWlibS1pbnRlbC1jb3Jwb3JhdGlvbi1zYW1zdW5nLzkwNzI2L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>ldentity Assurance Technologies Market Is Expected to Boom- IBM, Microsoft, Oracle, Cisco – TIMC</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiiQFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9sZGVudGl0eS1hc3N1cmFuY2UtdGVjaG5vbG9naWVzLW1hcmtldC1pcy1leHBlY3RlZC10by1ib29tLWlibS1taWNyb3NvZnQtb3JhY2xlLWNpc2NvLzkxMTg1L9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Cybersecurity in Aerospace Market is Expected to Record the Massive Growth, with Prominent Key Players – Cisco ...</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiygFodHRwczovL3d3dy50aGVpbmRpYW5tb3ZpZWNoYW5uZWwuY29tL2F3YXJkcy9jeWJlcnNlY3VyaXR5LWluLWFlcm9zcGFjZS1tYXJrZXQtaXMtZXhwZWN0ZWQtdG8tcmVjb3JkLXRoZS1tYXNzaXZlLWdyb3d0aC13aXRoLXByb21pbmVudC1rZXktcGxheWVycy1jaXNjby1pYm0tcmF5dGhlb24tdGVjaG5vbG9naWVzLW5vcnRocm9wLWdydW1tYW4vOTA3OTcv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Distributed Cloud Storage System Market Future Analysis | IBM Corp., Amazon web services, Huawei</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>2024-06-16 23:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMieWh0dHA6Ly9hbW9yZS5uZy93b3JsZHdpZGUvMjkvZGlzdHJpYnV0ZWQtY2xvdWQtc3RvcmFnZS1zeXN0ZW0tbWFya2V0LWZ1dHVyZS1hbmFseXNpcy1pYm0tY29ycC1hbWF6b24td2ViLXNlcnZpY2VzLWh1YXdlaS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Cloud Banking Service Industry Research Study |Mambu, Amazon Web Services, IBM</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:15:06.718936</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiaWh0dHA6Ly9hbW9yZS5uZy93b3JsZHdpZGUvNTQvY2xvdWQtYmFua2luZy1zZXJ2aWNlLWluZHVzdHJ5LXJlc2VhcmNoLXN0dWR5LW1hbWJ1LWFtYXpvbi13ZWItc2VydmljZXMtaWJtL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Internet Sanitation Service Market Future Analysis | The Noledge Group, IBM, Zhejiang Lianyun Zhihui SCI-tech</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiiAFodHRwczovL2Ftb3JlLm5nL3dvcmxkd2lkZS81NS9pbnRlcm5ldC1zYW5pdGF0aW9uLXNlcnZpY2UtbWFya2V0LWZ1dHVyZS1hbmFseXNpcy10aGUtbm9sZWRnZS1ncm91cC1pYm0temhlamlhbmctbGlhbnl1bi16aGlodWktc2NpLXRlY2gv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Consumer IAM Solutions Industry Research Study |IBM, Microsoft, Salesforce</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.376213</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZWh0dHA6Ly9hbW9yZS5uZy93b3JsZHdpZGUvNDAvY29uc3VtZXItaWFtLXNvbHV0aW9ucy1pbmR1c3RyeS1yZXNlYXJjaC1zdHVkeS1pYm0tbWljcm9zb2Z0LXNhbGVzZm9yY2Uv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>AI-Based Dynamic Pricing Tool Market Growth Drivers | IBM, McKinsey, Blue Yonder</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiZWh0dHA6Ly9hbW9yZS5uZy9uZXdzLzE2L2FpLWJhc2VkLWR5bmFtaWMtcHJpY2luZy10b29sLW1hcmtldC1ncm93dGgtZHJpdmVycy1pYm0tbWNraW5zZXktYmx1ZS15b25kZXIv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Live Production and Video Streaming Software Market Emerging Trends | IBM, Kaltura, BrightCove</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMic2h0dHA6Ly9hbW9yZS5uZy9uZXdzLzM1L2xpdmUtcHJvZHVjdGlvbi1hbmQtdmlkZW8tc3RyZWFtaW5nLXNvZnR3YXJlLW1hcmtldC1lbWVyZ2luZy10cmVuZHMtaWJtLWthbHR1cmEtYnJpZ2h0Y292ZS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Digital Commerce Price Optimization Software Market Research Report | SAP, IBM, Oracle</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMia2h0dHA6Ly9hbW9yZS5uZy9uZXdzLzM2L2RpZ2l0YWwtY29tbWVyY2UtcHJpY2Utb3B0aW1pemF0aW9uLXNvZnR3YXJlLW1hcmtldC1yZXNlYXJjaC1yZXBvcnQtc2FwLWlibS1vcmFjbGUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>IT safety: Vulnerable Linux, MacOS X and Windows - Eclipse Jetty IT safety alert replace (vulnerability: medium)</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMilQFodHRwczovL3d3dy5icmVha2luZ2xhdGVzdC5uZXdzL3RlY2hub2xvZ3kvaXQtc2FmZXR5LXZ1bG5lcmFibGUtbGludXgtbWFjb3MteC1hbmQtd2luZG93cy1lY2xpcHNlLWpldHR5LWl0LXNhZmV0eS1hbGVydC1yZXBsYWNlLXZ1bG5lcmFiaWxpdHktbWVkaXVtL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Advanced Server Energy Monitoring Software Market Trends and Regional Analysis | HP, IBM, Sun Microsystems</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMihAFodHRwOi8vYW1vcmUubmcvd29ybGR3aWRlLzM3L2FkdmFuY2VkLXNlcnZlci1lbmVyZ3ktbW9uaXRvcmluZy1zb2Z0d2FyZS1tYXJrZXQtdHJlbmRzLWFuZC1yZWdpb25hbC1hbmFseXNpcy1ocC1pYm0tc3VuLW1pY3Jvc3lzdGVtcy_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>Digital Forensic Software Market Emerging Trends | IBM, AccessData, FireEye</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiYGh0dHA6Ly9hbW9yZS5uZy9uZXdzLzMxL2RpZ2l0YWwtZm9yZW5zaWMtc29mdHdhcmUtbWFya2V0LWVtZXJnaW5nLXRyZW5kcy1pYm0tYWNjZXNzZGF0YS1maXJlZXllL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Version Control Clients System Market Growth Drivers | SourceTree, GitKraken, IBM Rational Team Concert</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifGh0dHA6Ly9hbW9yZS5uZy9uZXdzLzM3L3ZlcnNpb24tY29udHJvbC1jbGllbnRzLXN5c3RlbS1tYXJrZXQtZ3Jvd3RoLWRyaXZlcnMtc291cmNldHJlZS1naXRrcmFrZW4taWJtLXJhdGlvbmFsLXRlYW0tY29uY2VydC_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>Facilities Management and Workspace Solutions Market Trends and Regional Analysis | IBM, Oracle, SAP</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>2024-06-17 00:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMifmh0dHA6Ly9hbW9yZS5uZy93b3JsZHdpZGUvMzQvZmFjaWxpdGllcy1tYW5hZ2VtZW50LWFuZC13b3Jrc3BhY2Utc29sdXRpb25zLW1hcmtldC10cmVuZHMtYW5kLXJlZ2lvbmFsLWFuYWx5c2lzLWlibS1vcmFjbGUtc2FwL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>Metasearch Engine Industry Research Study |Dogpile, InfoSpace, IBM</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:15:06.718936</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiXmh0dHBzOi8vYW1vcmUubmcvd29ybGR3aWRlLzM4L21ldGFzZWFyY2gtZW5naW5lLWluZHVzdHJ5LXJlc2VhcmNoLXN0dWR5LWRvZ3BpbGUtaW5mb3NwYWNlLWlibS_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>IBM UK &amp; Ireland CEO Nicola Hodson on the AI revolution in business - How to be a CEO podcast</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiQWh0dHBzOi8vc2cubmV3cy55YWhvby5jb20vaWJtLWNlby1uaWNvbGEtaG9kc29uLWFpLTA4MDAzNjY3MS5odG1s0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>IBM and Wimbledon Launch AI Feature for Player Stories</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.371495</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiXWh0dHBzOi8vd3d3LmNyeXB0b3RpbWVzLmlvLzIwMjQvMDYvMTcvaWJtLWFuZC13aW1ibGVkb24tbGF1bmNoLWFpLWZlYXR1cmUtZm9yLXBsYXllci1zdG9yaWVzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Banking Security Market Emerging Trends | OneSpan, IBM Corporation, AO Kaspersky Lab.</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiamh0dHBzOi8vYW1vcmUubmcvbmV3cy8xNy9iYW5raW5nLXNlY3VyaXR5LW1hcmtldC1lbWVyZ2luZy10cmVuZHMtb25lc3Bhbi1pYm0tY29ycG9yYXRpb24tYW8ta2FzcGVyc2t5LWxhYi_SAQA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Data Asset Management Market [2024] | Anmut, IBM, Adobe</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiUGh0dHBzOi8vYW1vcmUubmcvd29ybGR3aWRlLzQ0L2RhdGEtYXNzZXQtbWFuYWdlbWVudC1tYXJrZXQtMjAyNC1hbm11dC1pYm0tYWRvYmUv0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>ModelOps Platforms Market Future Analysis | ModelOp, Modzy, IBM</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiWWh0dHA6Ly9hbW9yZS5uZy93b3JsZHdpZGUvMTMvbW9kZWxvcHMtcGxhdGZvcm1zLW1hcmtldC1mdXR1cmUtYW5hbHlzaXMtbW9kZWxvcC1tb2R6eS1pYm0v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Corporate Performance Management Software Market Report | Oracle, SAP, IBM</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMiX2h0dHA6Ly9hbW9yZS5uZy9uZXdzLzQwL2NvcnBvcmF0ZS1wZXJmb3JtYW5jZS1tYW5hZ2VtZW50LXNvZnR3YXJlLW1hcmtldC1yZXBvcnQtb3JhY2xlLXNhcC1pYm0v0gEA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>Intelligent Document Processing System Market Trends and Regional Analysis | IBM, OpenText, Datamatics</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>2024-06-17 01:33:47.377339</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>news.google.com/articles/CBMigAFodHRwOi8vYW1vcmUubmcvd29ybGR3aWRlLzQyL2ludGVsbGlnZW50LWRvY3VtZW50LXByb2Nlc3Npbmctc3lzdGVtLW1hcmtldC10cmVuZHMtYW5kLXJlZ2lvbmFsLWFuYWx5c2lzLWlibS1vcGVudGV4dC1kYXRhbWF0aWNzL9IBAA?hl=en-CA&amp;gl=CA&amp;ceid=CA%3Aen</t>
         </is>
       </c>
     </row>

</xml_diff>